<commit_message>
added some recall/precision table in excel sheet
</commit_message>
<xml_diff>
--- a/cob_surface_classification/common/files/experiments.xlsx
+++ b/cob_surface_classification/common/files/experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="206" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="206" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="158">
   <si>
     <t>parameters</t>
   </si>
@@ -564,6 +564,33 @@
   <si>
     <t>n/a</t>
   </si>
+  <si>
+    <t>Avg. recall</t>
+  </si>
+  <si>
+    <t>Gauss</t>
+  </si>
+  <si>
+    <t>Bilateral</t>
+  </si>
+  <si>
+    <t>Avg. recall/precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>Avg. precision</t>
+  </si>
 </sst>
 </file>
 
@@ -572,7 +599,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -618,6 +645,14 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -660,10 +695,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -678,8 +714,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1284,10 +1322,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="B2:AU663"/>
+  <dimension ref="B2:CE663"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I192" sqref="I192"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BL24" sqref="BL24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1313,7 +1351,7 @@
     <col min="41" max="1007" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:66">
       <c r="K2" t="s">
         <v>41</v>
       </c>
@@ -1321,7 +1359,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:66">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1332,12 +1370,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:66">
       <c r="K4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:66">
       <c r="C5" t="s">
         <v>46</v>
       </c>
@@ -1345,12 +1383,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:66">
       <c r="K6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:66">
       <c r="D7" t="s">
         <v>49</v>
       </c>
@@ -1358,7 +1396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:66">
       <c r="C8" t="s">
         <v>51</v>
       </c>
@@ -1366,46 +1404,331 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:66">
       <c r="K9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:66">
       <c r="J11" t="s">
         <v>54</v>
       </c>
       <c r="K11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="2:12">
+      <c r="AZ11" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>45</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>48</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>52</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:66">
       <c r="K12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="2:12">
+      <c r="AZ12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BL12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="2:66">
+      <c r="AX13">
+        <v>10</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ13" s="6">
+        <v>91.174553333333321</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB13" s="6">
+        <v>88.889213333333316</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD13" s="6">
+        <v>87.04676666666667</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF13" s="6">
+        <v>83.986646666666658</v>
+      </c>
+      <c r="BG13" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH13" s="6">
+        <v>89.606246666666678</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ13" s="6">
+        <v>87.897593333333333</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL13" s="6">
+        <v>85.256526666666659</v>
+      </c>
+      <c r="BM13" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN13" s="6"/>
+    </row>
+    <row r="14" spans="2:66">
       <c r="J14" t="s">
         <v>57</v>
       </c>
       <c r="K14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="2:12">
+      <c r="AW14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ14" s="6">
+        <v>84.680472380952381</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB14" s="6">
+        <v>86.663540000000012</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD14" s="6">
+        <v>85.754426666666674</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF14" s="6">
+        <v>80.272293333333351</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH14" s="6">
+        <v>86.326180000000008</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ14" s="6">
+        <v>86.499846666666656</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL14" s="6">
+        <v>83.538353333333333</v>
+      </c>
+      <c r="BM14" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN14" s="6"/>
+    </row>
+    <row r="15" spans="2:66">
       <c r="J15" t="s">
         <v>58</v>
       </c>
       <c r="K15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="2:12">
+      <c r="AX15">
+        <v>15</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ15" s="6">
+        <v>90.422006666666661</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB15" s="6">
+        <v>87.987053333333321</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD15" s="6">
+        <v>86.01936666666667</v>
+      </c>
+      <c r="BE15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF15" s="6">
+        <v>82.851166666666671</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH15" s="6">
+        <v>88.768679999999989</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ15" s="6">
+        <v>86.929346666666632</v>
+      </c>
+      <c r="BK15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL15" s="6">
+        <v>84.186066666666676</v>
+      </c>
+      <c r="BM15" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="2:66">
       <c r="K16">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="10:39">
+      <c r="AY16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ16" s="6">
+        <v>85.40446</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB16" s="6">
+        <v>87.42800666666669</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD16" s="6">
+        <v>86.117226666666667</v>
+      </c>
+      <c r="BE16" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF16" s="6">
+        <v>80.617593333333332</v>
+      </c>
+      <c r="BG16" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH16" s="6">
+        <v>87.422679999999986</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ16" s="6">
+        <v>87.01196666666668</v>
+      </c>
+      <c r="BK16" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL16" s="6">
+        <v>83.810586666666666</v>
+      </c>
+      <c r="BM16" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="10:83">
+      <c r="AX17">
+        <v>20</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ17" s="6">
+        <v>89.775120000000015</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB17" s="6">
+        <v>87.20999333333333</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD17" s="6">
+        <v>85.240666666666655</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF17" s="6">
+        <v>81.958826666666667</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH17" s="6">
+        <v>88.014206666666681</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ17" s="6">
+        <v>86.138979999999989</v>
+      </c>
+      <c r="BK17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL17" s="6">
+        <v>83.308680000000024</v>
+      </c>
+      <c r="BM17" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="10:83">
       <c r="J18" t="s">
         <v>59</v>
       </c>
@@ -1418,8 +1741,54 @@
       <c r="AC18" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="10:39">
+      <c r="AY18" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ18" s="6">
+        <v>85.641422857142842</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB18" s="6">
+        <v>87.55398666666666</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD18" s="6">
+        <v>86.176086666666649</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF18" s="6">
+        <v>81.161293333333333</v>
+      </c>
+      <c r="BG18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH18" s="6">
+        <v>87.62103333333333</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ18" s="6">
+        <v>87.089320000000015</v>
+      </c>
+      <c r="BK18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL18" s="6">
+        <v>83.961793333333347</v>
+      </c>
+      <c r="BM18" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN18" s="6"/>
+    </row>
+    <row r="19" spans="10:83">
       <c r="K19">
         <v>45</v>
       </c>
@@ -1469,8 +1838,57 @@
       <c r="AJ19" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="10:39">
+      <c r="AX19">
+        <v>35</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ19" s="6">
+        <v>90.945119999999989</v>
+      </c>
+      <c r="BA19" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB19" s="6">
+        <v>88.65506000000002</v>
+      </c>
+      <c r="BC19" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD19" s="6">
+        <v>86.783519999999996</v>
+      </c>
+      <c r="BE19" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF19" s="6">
+        <v>83.67397333333335</v>
+      </c>
+      <c r="BG19" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH19" s="6">
+        <v>89.388080000000002</v>
+      </c>
+      <c r="BI19" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ19" s="6">
+        <v>87.648973333333331</v>
+      </c>
+      <c r="BK19" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL19" s="6">
+        <v>84.977419999999981</v>
+      </c>
+      <c r="BM19" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN19" s="6"/>
+    </row>
+    <row r="20" spans="10:83">
       <c r="K20">
         <v>60</v>
       </c>
@@ -1525,8 +1943,57 @@
         <v>85.429122877256646</v>
       </c>
       <c r="AK20" s="6"/>
-    </row>
-    <row r="21" spans="10:39">
+      <c r="AW20" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ20" s="6">
+        <v>82.379989523809513</v>
+      </c>
+      <c r="BA20" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB20" s="6">
+        <v>84.340206666666674</v>
+      </c>
+      <c r="BC20" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD20" s="6">
+        <v>83.510613333333339</v>
+      </c>
+      <c r="BE20" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF20" s="6">
+        <v>77.69913333333335</v>
+      </c>
+      <c r="BG20" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH20" s="6">
+        <v>83.968979999999974</v>
+      </c>
+      <c r="BI20" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ20" s="6">
+        <v>84.253266666666661</v>
+      </c>
+      <c r="BK20" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL20" s="6">
+        <v>81.278346666666692</v>
+      </c>
+      <c r="BM20" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN20" s="6"/>
+    </row>
+    <row r="21" spans="10:83">
       <c r="R21" s="8" t="s">
         <v>96</v>
       </c>
@@ -1582,8 +2049,56 @@
         <v>84.878510849849945</v>
       </c>
       <c r="AK21" s="6"/>
-    </row>
-    <row r="22" spans="10:39">
+      <c r="AX21">
+        <v>45</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ21" s="6">
+        <v>90.551246666666671</v>
+      </c>
+      <c r="BA21" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB21" s="6">
+        <v>88.154046666666673</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD21" s="6">
+        <v>86.248826666666687</v>
+      </c>
+      <c r="BE21" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF21" s="6">
+        <v>83.097253333333342</v>
+      </c>
+      <c r="BG21" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH21" s="6">
+        <v>88.91467333333334</v>
+      </c>
+      <c r="BI21" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ21" s="6">
+        <v>87.125386666666657</v>
+      </c>
+      <c r="BK21" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL21" s="6">
+        <v>84.397473333333338</v>
+      </c>
+      <c r="BM21" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="10:83">
       <c r="J22" t="s">
         <v>60</v>
       </c>
@@ -1641,8 +2156,53 @@
         <v>84.399809446876489</v>
       </c>
       <c r="AK22" s="6"/>
-    </row>
-    <row r="23" spans="10:39">
+      <c r="AY22" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ22" s="6">
+        <v>85.348445714285717</v>
+      </c>
+      <c r="BA22" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB22" s="6">
+        <v>87.43874000000001</v>
+      </c>
+      <c r="BC22" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD22" s="6">
+        <v>86.088379999999987</v>
+      </c>
+      <c r="BE22" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF22" s="6">
+        <v>80.589506666666665</v>
+      </c>
+      <c r="BG22" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH22" s="6">
+        <v>87.395320000000012</v>
+      </c>
+      <c r="BI22" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ22" s="6">
+        <v>86.997553333333343</v>
+      </c>
+      <c r="BK22" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL22" s="6">
+        <v>83.700426666666672</v>
+      </c>
+      <c r="BM22" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="10:83">
       <c r="K23">
         <v>5.0000000000000001E-4</v>
       </c>
@@ -1697,8 +2257,56 @@
         <v>83.855043198213409</v>
       </c>
       <c r="AK23" s="6"/>
-    </row>
-    <row r="24" spans="10:39">
+      <c r="AX23">
+        <v>60</v>
+      </c>
+      <c r="AY23" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ23" s="6">
+        <v>89.875313333333324</v>
+      </c>
+      <c r="BA23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB23" s="6">
+        <v>87.277153333333345</v>
+      </c>
+      <c r="BC23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD23" s="6">
+        <v>85.274453333333341</v>
+      </c>
+      <c r="BE23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF23" s="6">
+        <v>82.025413333333347</v>
+      </c>
+      <c r="BG23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH23" s="6">
+        <v>88.086380000000005</v>
+      </c>
+      <c r="BI23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ23" s="6">
+        <v>86.191559999999996</v>
+      </c>
+      <c r="BK23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL23" s="6">
+        <v>83.376379999999997</v>
+      </c>
+      <c r="BM23" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="10:83">
       <c r="K24">
         <v>1E-3</v>
       </c>
@@ -1757,8 +2365,54 @@
         <v>84.684906295635955</v>
       </c>
       <c r="AK24" s="6"/>
-    </row>
-    <row r="25" spans="10:39">
+      <c r="AY24" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ24" s="6">
+        <v>87.997920000000008</v>
+      </c>
+      <c r="BA24" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB24" s="6">
+        <v>89.866586666666677</v>
+      </c>
+      <c r="BC24" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD24" s="6">
+        <v>88.448746666666651</v>
+      </c>
+      <c r="BE24" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF24" s="6">
+        <v>83.762540000000001</v>
+      </c>
+      <c r="BG24" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH24" s="6">
+        <v>90.005593333333323</v>
+      </c>
+      <c r="BI24" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ24" s="6">
+        <v>89.350313333333332</v>
+      </c>
+      <c r="BK24" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL24" s="6">
+        <v>86.331960000000009</v>
+      </c>
+      <c r="BM24" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN24" s="6"/>
+    </row>
+    <row r="25" spans="10:83">
       <c r="K25">
         <v>2E-3</v>
       </c>
@@ -1814,12 +2468,12 @@
       </c>
       <c r="AK25" s="6"/>
     </row>
-    <row r="26" spans="10:39">
+    <row r="26" spans="10:83">
       <c r="K26">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="10:39">
+    <row r="30" spans="10:83">
       <c r="O30" s="5" t="s">
         <v>61</v>
       </c>
@@ -1872,8 +2526,104 @@
         <v>64</v>
       </c>
       <c r="AM30" s="5"/>
-    </row>
-    <row r="31" spans="10:39">
+      <c r="AW30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ30" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA30">
+        <v>0</v>
+      </c>
+      <c r="BB30" t="s">
+        <v>45</v>
+      </c>
+      <c r="BC30">
+        <v>1</v>
+      </c>
+      <c r="BD30" t="s">
+        <v>47</v>
+      </c>
+      <c r="BE30">
+        <v>1</v>
+      </c>
+      <c r="BF30" t="s">
+        <v>48</v>
+      </c>
+      <c r="BG30">
+        <v>1</v>
+      </c>
+      <c r="BH30" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI30">
+        <v>2</v>
+      </c>
+      <c r="BJ30" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK30">
+        <v>2</v>
+      </c>
+      <c r="BL30" t="s">
+        <v>53</v>
+      </c>
+      <c r="BM30">
+        <v>2</v>
+      </c>
+      <c r="BO30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BP30" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR30" t="s">
+        <v>63</v>
+      </c>
+      <c r="BS30">
+        <v>0</v>
+      </c>
+      <c r="BT30" t="s">
+        <v>45</v>
+      </c>
+      <c r="BU30">
+        <v>1</v>
+      </c>
+      <c r="BV30" t="s">
+        <v>47</v>
+      </c>
+      <c r="BW30">
+        <v>1</v>
+      </c>
+      <c r="BX30" t="s">
+        <v>48</v>
+      </c>
+      <c r="BY30">
+        <v>1</v>
+      </c>
+      <c r="BZ30" t="s">
+        <v>50</v>
+      </c>
+      <c r="CA30">
+        <v>2</v>
+      </c>
+      <c r="CB30" t="s">
+        <v>52</v>
+      </c>
+      <c r="CC30">
+        <v>2</v>
+      </c>
+      <c r="CD30" t="s">
+        <v>53</v>
+      </c>
+      <c r="CE30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="10:83">
       <c r="S31">
         <v>3</v>
       </c>
@@ -1898,8 +2648,50 @@
       <c r="AG31" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="10:39">
+      <c r="BA31">
+        <v>3</v>
+      </c>
+      <c r="BC31">
+        <v>3</v>
+      </c>
+      <c r="BE31">
+        <v>5</v>
+      </c>
+      <c r="BG31">
+        <v>7</v>
+      </c>
+      <c r="BI31">
+        <v>3</v>
+      </c>
+      <c r="BK31">
+        <v>5</v>
+      </c>
+      <c r="BM31">
+        <v>7</v>
+      </c>
+      <c r="BS31">
+        <v>3</v>
+      </c>
+      <c r="BU31">
+        <v>3</v>
+      </c>
+      <c r="BW31">
+        <v>5</v>
+      </c>
+      <c r="BY31">
+        <v>7</v>
+      </c>
+      <c r="CA31">
+        <v>3</v>
+      </c>
+      <c r="CC31">
+        <v>5</v>
+      </c>
+      <c r="CE31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="10:83">
       <c r="P32" t="s">
         <v>66</v>
       </c>
@@ -1948,8 +2740,56 @@
       <c r="AE32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="3:47">
+      <c r="AX32" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BD32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BF32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BH32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BJ32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BL32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BP32" t="s">
+        <v>157</v>
+      </c>
+      <c r="BR32" t="s">
+        <v>157</v>
+      </c>
+      <c r="BT32" t="s">
+        <v>157</v>
+      </c>
+      <c r="BV32" t="s">
+        <v>157</v>
+      </c>
+      <c r="BX32" t="s">
+        <v>157</v>
+      </c>
+      <c r="BZ32" t="s">
+        <v>157</v>
+      </c>
+      <c r="CB32" t="s">
+        <v>157</v>
+      </c>
+      <c r="CD32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="3:83">
       <c r="C33" t="s">
         <v>68</v>
       </c>
@@ -1980,8 +2820,14 @@
       <c r="O33" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="3:47">
+      <c r="AW33" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="3:83">
       <c r="C34">
         <v>0</v>
       </c>
@@ -2084,8 +2930,94 @@
       <c r="AN34" s="6"/>
       <c r="AO34" s="6"/>
       <c r="AP34" s="6"/>
-    </row>
-    <row r="35" spans="3:47">
+      <c r="AW34">
+        <v>0</v>
+      </c>
+      <c r="AX34" s="6">
+        <f t="array" ref="AX34">AVERAGEIF($F$34:$F$663,AW34,$I$34:$I$663)</f>
+        <v>85.253000317460291</v>
+      </c>
+      <c r="AY34" s="6"/>
+      <c r="AZ34" s="6">
+        <f t="array" ref="AZ34">AVERAGE(IF(($D$34:$D$663=BA$30)*($E$34:$E$663=BA$31)*($F$34:$F$663=AW34),$I$34:$I$663))</f>
+        <v>89.185442222222207</v>
+      </c>
+      <c r="BA34" s="6"/>
+      <c r="BB34" s="6">
+        <f t="array" ref="BB34">AVERAGE(IF(($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($F$34:$F$663=AW34),$I$34:$I$663))</f>
+        <v>86.450595555555552</v>
+      </c>
+      <c r="BC34" s="6"/>
+      <c r="BD34" s="6">
+        <f t="array" ref="BD34">AVERAGE(IF(($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($F$34:$F$663=AW34),$I$34:$I$663))</f>
+        <v>84.472184444444451</v>
+      </c>
+      <c r="BE34" s="6"/>
+      <c r="BF34" s="6">
+        <f t="array" ref="BF34">AVERAGE(IF(($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($F$34:$F$663=AW34),$I$34:$I$663))</f>
+        <v>81.374488888888877</v>
+      </c>
+      <c r="BG34" s="6"/>
+      <c r="BH34" s="6">
+        <f t="array" ref="BH34">AVERAGE(IF(($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($F$34:$F$663=AW34),$I$34:$I$663))</f>
+        <v>87.275480000000016</v>
+      </c>
+      <c r="BI34" s="6"/>
+      <c r="BJ34" s="6">
+        <f t="array" ref="BJ34">AVERAGE(IF(($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($F$34:$F$663=AW34),$I$34:$I$663))</f>
+        <v>85.374571111111095</v>
+      </c>
+      <c r="BK34" s="6"/>
+      <c r="BL34" s="6">
+        <f t="array" ref="BL34">AVERAGE(IF(($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($F$34:$F$663=AW34),$I$34:$I$663))</f>
+        <v>82.63824000000001</v>
+      </c>
+      <c r="BM34" s="6"/>
+      <c r="BO34">
+        <v>0</v>
+      </c>
+      <c r="BP34" s="6">
+        <f t="array" ref="BP34">AVERAGEIF($F$34:$F$663,BO34,$J$34:$J$663)</f>
+        <v>85.750123174603175</v>
+      </c>
+      <c r="BQ34" s="6"/>
+      <c r="BR34" s="6">
+        <f t="array" ref="BR34">AVERAGE(IF(($D$34:$D$663=BS$30)*($E$34:$E$663=BS$31)*($F$34:$F$663=BO34),$J$34:$J$663))</f>
+        <v>84.404728888888869</v>
+      </c>
+      <c r="BS34" s="6"/>
+      <c r="BT34" s="6">
+        <f t="array" ref="BT34">AVERAGE(IF(($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($F$34:$F$663=BO34),$J$34:$J$663))</f>
+        <v>87.343155555555555</v>
+      </c>
+      <c r="BU34" s="6"/>
+      <c r="BV34" s="6">
+        <f t="array" ref="BV34">AVERAGE(IF(($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($F$34:$F$663=BO34),$J$34:$J$663))</f>
+        <v>86.60652222222221</v>
+      </c>
+      <c r="BW34" s="6"/>
+      <c r="BX34" s="6">
+        <f t="array" ref="BX34">AVERAGE(IF(($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($F$34:$F$663=BO34),$J$34:$J$663))</f>
+        <v>82.791377777777797</v>
+      </c>
+      <c r="BY34" s="6"/>
+      <c r="BZ34" s="6">
+        <f t="array" ref="BZ34">AVERAGE(IF(($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($F$34:$F$663=BO34),$J$34:$J$663))</f>
+        <v>87.037422222222219</v>
+      </c>
+      <c r="CA34" s="6"/>
+      <c r="CB34" s="6">
+        <f t="array" ref="CB34">AVERAGE(IF(($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($F$34:$F$663=BO34),$J$34:$J$663))</f>
+        <v>87.194468888888892</v>
+      </c>
+      <c r="CC34" s="6"/>
+      <c r="CD34" s="6">
+        <f t="array" ref="CD34">AVERAGE(IF(($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($F$34:$F$663=BO34),$J$34:$J$663))</f>
+        <v>84.873186666666655</v>
+      </c>
+      <c r="CE34" s="6"/>
+    </row>
+    <row r="35" spans="3:83">
       <c r="C35">
         <v>5.0000000000000001E-4</v>
       </c>
@@ -2191,8 +3123,94 @@
       <c r="AN35" s="6"/>
       <c r="AO35" s="6"/>
       <c r="AP35" s="6"/>
-    </row>
-    <row r="36" spans="3:47">
+      <c r="AW35">
+        <v>1</v>
+      </c>
+      <c r="AX35" s="6">
+        <f t="array" ref="AX35">AVERAGEIF($F$34:$F$663,AW35,$I$34:$I$663)</f>
+        <v>86.793700317460392</v>
+      </c>
+      <c r="AY35" s="6"/>
+      <c r="AZ35" s="6">
+        <f t="array" ref="AZ35">AVERAGE(IF(($D$34:$D$663=BA$30)*($E$34:$E$663=BA$31)*($F$34:$F$663=AW35),$I$34:$I$663))</f>
+        <v>90.457226666666642</v>
+      </c>
+      <c r="BA35" s="6"/>
+      <c r="BB35" s="6">
+        <f t="array" ref="BB35">AVERAGE(IF(($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($F$34:$F$663=AW35),$I$34:$I$663))</f>
+        <v>88.028753333333341</v>
+      </c>
+      <c r="BC35" s="6"/>
+      <c r="BD35" s="6">
+        <f t="array" ref="BD35">AVERAGE(IF(($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($F$34:$F$663=AW35),$I$34:$I$663))</f>
+        <v>86.102266666666665</v>
+      </c>
+      <c r="BE35" s="6"/>
+      <c r="BF35" s="6">
+        <f t="array" ref="BF35">AVERAGE(IF(($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($F$34:$F$663=AW35),$I$34:$I$663))</f>
+        <v>82.932213333333337</v>
+      </c>
+      <c r="BG35" s="6"/>
+      <c r="BH35" s="6">
+        <f t="array" ref="BH35">AVERAGE(IF(($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($F$34:$F$663=AW35),$I$34:$I$663))</f>
+        <v>88.796377777777792</v>
+      </c>
+      <c r="BI35" s="6"/>
+      <c r="BJ35" s="6">
+        <f t="array" ref="BJ35">AVERAGE(IF(($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($F$34:$F$663=AW35),$I$34:$I$663))</f>
+        <v>86.988639999999975</v>
+      </c>
+      <c r="BK35" s="6"/>
+      <c r="BL35" s="6">
+        <f t="array" ref="BL35">AVERAGE(IF(($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($F$34:$F$663=AW35),$I$34:$I$663))</f>
+        <v>84.250424444444462</v>
+      </c>
+      <c r="BM35" s="6"/>
+      <c r="BO35">
+        <v>1</v>
+      </c>
+      <c r="BP35" s="6">
+        <f t="array" ref="BP35">AVERAGEIF($F$34:$F$663,BO35,$J$34:$J$663)</f>
+        <v>85.24211841269846</v>
+      </c>
+      <c r="BQ35" s="6"/>
+      <c r="BR35" s="6">
+        <f t="array" ref="BR35">AVERAGE(IF(($D$34:$D$663=BS$30)*($E$34:$E$663=BS$31)*($F$34:$F$663=BO35),$J$34:$J$663))</f>
+        <v>85.019424444444439</v>
+      </c>
+      <c r="BS35" s="6"/>
+      <c r="BT35" s="6">
+        <f t="array" ref="BT35">AVERAGE(IF(($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($F$34:$F$663=BO35),$J$34:$J$663))</f>
+        <v>87.215177777777797</v>
+      </c>
+      <c r="BU35" s="6"/>
+      <c r="BV35" s="6">
+        <f t="array" ref="BV35">AVERAGE(IF(($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($F$34:$F$663=BO35),$J$34:$J$663))</f>
+        <v>86.015913333333373</v>
+      </c>
+      <c r="BW35" s="6"/>
+      <c r="BX35" s="6">
+        <f t="array" ref="BX35">AVERAGE(IF(($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($F$34:$F$663=BO35),$J$34:$J$663))</f>
+        <v>80.683726666666701</v>
+      </c>
+      <c r="BY35" s="6"/>
+      <c r="BZ35" s="6">
+        <f t="array" ref="BZ35">AVERAGE(IF(($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($F$34:$F$663=BO35),$J$34:$J$663))</f>
+        <v>87.123297777777765</v>
+      </c>
+      <c r="CA35" s="6"/>
+      <c r="CB35" s="6">
+        <f t="array" ref="CB35">AVERAGE(IF(($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($F$34:$F$663=BO35),$J$34:$J$663))</f>
+        <v>86.86704444444446</v>
+      </c>
+      <c r="CC35" s="6"/>
+      <c r="CD35" s="6">
+        <f t="array" ref="CD35">AVERAGE(IF(($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($F$34:$F$663=BO35),$J$34:$J$663))</f>
+        <v>83.770244444444458</v>
+      </c>
+      <c r="CE35" s="6"/>
+    </row>
+    <row r="36" spans="3:83">
       <c r="C36">
         <v>1E-3</v>
       </c>
@@ -2241,8 +3259,46 @@
       <c r="AC36" s="6"/>
       <c r="AD36" s="6"/>
       <c r="AE36" s="6"/>
-    </row>
-    <row r="37" spans="3:47">
+      <c r="AP36" t="s">
+        <v>150</v>
+      </c>
+      <c r="AS36" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX36" s="6"/>
+      <c r="AY36" s="6"/>
+      <c r="AZ36" s="6"/>
+      <c r="BA36" s="6"/>
+      <c r="BB36" s="6"/>
+      <c r="BC36" s="6"/>
+      <c r="BD36" s="6"/>
+      <c r="BE36" s="6"/>
+      <c r="BF36" s="6"/>
+      <c r="BG36" s="6"/>
+      <c r="BH36" s="6"/>
+      <c r="BI36" s="6"/>
+      <c r="BJ36" s="6"/>
+      <c r="BK36" s="6"/>
+      <c r="BL36" s="6"/>
+      <c r="BM36" s="6"/>
+      <c r="BP36" s="6"/>
+      <c r="BQ36" s="6"/>
+      <c r="BR36" s="6"/>
+      <c r="BS36" s="6"/>
+      <c r="BT36" s="6"/>
+      <c r="BU36" s="6"/>
+      <c r="BV36" s="6"/>
+      <c r="BW36" s="6"/>
+      <c r="BX36" s="6"/>
+      <c r="BY36" s="6"/>
+      <c r="BZ36" s="6"/>
+      <c r="CA36" s="6"/>
+      <c r="CB36" s="6"/>
+      <c r="CC36" s="6"/>
+      <c r="CD36" s="6"/>
+      <c r="CE36" s="6"/>
+    </row>
+    <row r="37" spans="3:83">
       <c r="C37">
         <v>2E-3</v>
       </c>
@@ -2312,8 +3368,40 @@
       <c r="AU37">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="3:47">
+      <c r="AX37" s="6"/>
+      <c r="AY37" s="6"/>
+      <c r="AZ37" s="6"/>
+      <c r="BA37" s="6"/>
+      <c r="BB37" s="6"/>
+      <c r="BC37" s="6"/>
+      <c r="BD37" s="6"/>
+      <c r="BE37" s="6"/>
+      <c r="BF37" s="6"/>
+      <c r="BG37" s="6"/>
+      <c r="BH37" s="6"/>
+      <c r="BI37" s="6"/>
+      <c r="BJ37" s="6"/>
+      <c r="BK37" s="6"/>
+      <c r="BL37" s="6"/>
+      <c r="BM37" s="6"/>
+      <c r="BP37" s="6"/>
+      <c r="BQ37" s="6"/>
+      <c r="BR37" s="6"/>
+      <c r="BS37" s="6"/>
+      <c r="BT37" s="6"/>
+      <c r="BU37" s="6"/>
+      <c r="BV37" s="6"/>
+      <c r="BW37" s="6"/>
+      <c r="BX37" s="6"/>
+      <c r="BY37" s="6"/>
+      <c r="BZ37" s="6"/>
+      <c r="CA37" s="6"/>
+      <c r="CB37" s="6"/>
+      <c r="CC37" s="6"/>
+      <c r="CD37" s="6"/>
+      <c r="CE37" s="6"/>
+    </row>
+    <row r="38" spans="3:83">
       <c r="C38">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -2386,8 +3474,46 @@
       <c r="AU38" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="3:47">
+      <c r="AW38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX38" s="6"/>
+      <c r="AY38" s="6"/>
+      <c r="AZ38" s="6"/>
+      <c r="BA38" s="6"/>
+      <c r="BB38" s="6"/>
+      <c r="BC38" s="6"/>
+      <c r="BD38" s="6"/>
+      <c r="BE38" s="6"/>
+      <c r="BF38" s="6"/>
+      <c r="BG38" s="6"/>
+      <c r="BH38" s="6"/>
+      <c r="BI38" s="6"/>
+      <c r="BJ38" s="6"/>
+      <c r="BK38" s="6"/>
+      <c r="BL38" s="6"/>
+      <c r="BM38" s="6"/>
+      <c r="BO38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BP38" s="6"/>
+      <c r="BQ38" s="6"/>
+      <c r="BR38" s="6"/>
+      <c r="BS38" s="6"/>
+      <c r="BT38" s="6"/>
+      <c r="BU38" s="6"/>
+      <c r="BV38" s="6"/>
+      <c r="BW38" s="6"/>
+      <c r="BX38" s="6"/>
+      <c r="BY38" s="6"/>
+      <c r="BZ38" s="6"/>
+      <c r="CA38" s="6"/>
+      <c r="CB38" s="6"/>
+      <c r="CC38" s="6"/>
+      <c r="CD38" s="6"/>
+      <c r="CE38" s="6"/>
+    </row>
+    <row r="39" spans="3:83">
       <c r="C39">
         <v>0</v>
       </c>
@@ -2511,8 +3637,94 @@
       <c r="AU39" s="6">
         <v>85.429122877256646</v>
       </c>
-    </row>
-    <row r="40" spans="3:47">
+      <c r="AW39">
+        <v>10</v>
+      </c>
+      <c r="AX39" s="6">
+        <f t="array" ref="AX39">AVERAGE(IF(($F$34:$F$663=AW35)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>87.693935238095236</v>
+      </c>
+      <c r="AY39" s="6"/>
+      <c r="AZ39" s="6">
+        <f t="array" ref="AZ39">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BA30)*($E$34:$E$663=BA31)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>91.174553333333321</v>
+      </c>
+      <c r="BA39" s="6"/>
+      <c r="BB39" s="6">
+        <f t="array" ref="BB39">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>88.889213333333316</v>
+      </c>
+      <c r="BC39" s="6"/>
+      <c r="BD39" s="6">
+        <f t="array" ref="BD39">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>87.04676666666667</v>
+      </c>
+      <c r="BE39" s="6"/>
+      <c r="BF39" s="6">
+        <f t="array" ref="BF39">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>83.986646666666658</v>
+      </c>
+      <c r="BG39" s="6"/>
+      <c r="BH39" s="6">
+        <f t="array" ref="BH39">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>89.606246666666678</v>
+      </c>
+      <c r="BI39" s="6"/>
+      <c r="BJ39" s="6">
+        <f t="array" ref="BJ39">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>87.897593333333333</v>
+      </c>
+      <c r="BK39" s="6"/>
+      <c r="BL39" s="6">
+        <f t="array" ref="BL39">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($G$34:$G$663=AW39),$I$34:$I$663))</f>
+        <v>85.256526666666659</v>
+      </c>
+      <c r="BM39" s="6"/>
+      <c r="BO39">
+        <v>10</v>
+      </c>
+      <c r="BP39" s="6">
+        <f t="array" ref="BP39">AVERAGE(IF(($F$34:$F$663=BO35)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>84.680472380952381</v>
+      </c>
+      <c r="BQ39" s="6"/>
+      <c r="BR39" s="6">
+        <f t="array" ref="BR39">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BS30)*($E$34:$E$663=BS31)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>83.708666666666659</v>
+      </c>
+      <c r="BS39" s="6"/>
+      <c r="BT39" s="6">
+        <f t="array" ref="BT39">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>86.663540000000012</v>
+      </c>
+      <c r="BU39" s="6"/>
+      <c r="BV39" s="6">
+        <f t="array" ref="BV39">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>85.754426666666674</v>
+      </c>
+      <c r="BW39" s="6"/>
+      <c r="BX39" s="6">
+        <f t="array" ref="BX39">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>80.272293333333351</v>
+      </c>
+      <c r="BY39" s="6"/>
+      <c r="BZ39" s="6">
+        <f t="array" ref="BZ39">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>86.326180000000008</v>
+      </c>
+      <c r="CA39" s="6"/>
+      <c r="CB39" s="6">
+        <f t="array" ref="CB39">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>86.499846666666656</v>
+      </c>
+      <c r="CC39" s="6"/>
+      <c r="CD39" s="6">
+        <f t="array" ref="CD39">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($G$34:$G$663=BO39),$J$34:$J$663))</f>
+        <v>83.538353333333333</v>
+      </c>
+      <c r="CE39" s="6"/>
+    </row>
+    <row r="40" spans="3:83">
       <c r="C40">
         <v>5.0000000000000001E-4</v>
       </c>
@@ -2639,8 +3851,94 @@
       <c r="AU40" s="6">
         <v>84.878510849849945</v>
       </c>
-    </row>
-    <row r="41" spans="3:47">
+      <c r="AW40">
+        <v>15</v>
+      </c>
+      <c r="AX40" s="6">
+        <f t="array" ref="AX40">AVERAGE(IF(($F$34:$F$663=AW35)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>86.737669523809501</v>
+      </c>
+      <c r="AY40" s="6"/>
+      <c r="AZ40" s="6">
+        <f t="array" ref="AZ40">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BA30)*($E$34:$E$663=BA31)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>90.422006666666661</v>
+      </c>
+      <c r="BA40" s="6"/>
+      <c r="BB40" s="6">
+        <f t="array" ref="BB40">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>87.987053333333321</v>
+      </c>
+      <c r="BC40" s="6"/>
+      <c r="BD40" s="6">
+        <f t="array" ref="BD40">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>86.01936666666667</v>
+      </c>
+      <c r="BE40" s="6"/>
+      <c r="BF40" s="6">
+        <f t="array" ref="BF40">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>82.851166666666671</v>
+      </c>
+      <c r="BG40" s="6"/>
+      <c r="BH40" s="6">
+        <f t="array" ref="BH40">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>88.768679999999989</v>
+      </c>
+      <c r="BI40" s="6"/>
+      <c r="BJ40" s="6">
+        <f t="array" ref="BJ40">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>86.929346666666632</v>
+      </c>
+      <c r="BK40" s="6"/>
+      <c r="BL40" s="6">
+        <f t="array" ref="BL40">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($G$34:$G$663=AW40),$I$34:$I$663))</f>
+        <v>84.186066666666676</v>
+      </c>
+      <c r="BM40" s="6"/>
+      <c r="BO40">
+        <v>15</v>
+      </c>
+      <c r="BP40" s="6">
+        <f t="array" ref="BP40">AVERAGE(IF(($F$34:$F$663=BO35)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>85.40446</v>
+      </c>
+      <c r="BQ40" s="6"/>
+      <c r="BR40" s="6">
+        <f t="array" ref="BR40">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BS30)*($E$34:$E$663=BS31)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>85.42316000000001</v>
+      </c>
+      <c r="BS40" s="6"/>
+      <c r="BT40" s="6">
+        <f t="array" ref="BT40">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>87.42800666666669</v>
+      </c>
+      <c r="BU40" s="6"/>
+      <c r="BV40" s="6">
+        <f t="array" ref="BV40">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>86.117226666666667</v>
+      </c>
+      <c r="BW40" s="6"/>
+      <c r="BX40" s="6">
+        <f t="array" ref="BX40">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>80.617593333333332</v>
+      </c>
+      <c r="BY40" s="6"/>
+      <c r="BZ40" s="6">
+        <f t="array" ref="BZ40">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>87.422679999999986</v>
+      </c>
+      <c r="CA40" s="6"/>
+      <c r="CB40" s="6">
+        <f t="array" ref="CB40">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>87.01196666666668</v>
+      </c>
+      <c r="CC40" s="6"/>
+      <c r="CD40" s="6">
+        <f t="array" ref="CD40">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($G$34:$G$663=BO40),$J$34:$J$663))</f>
+        <v>83.810586666666666</v>
+      </c>
+      <c r="CE40" s="6"/>
+    </row>
+    <row r="41" spans="3:83">
       <c r="C41">
         <v>1E-3</v>
       </c>
@@ -2764,8 +4062,94 @@
       <c r="AU41" s="6">
         <v>84.399809446876489</v>
       </c>
-    </row>
-    <row r="42" spans="3:47">
+      <c r="AW41">
+        <v>20</v>
+      </c>
+      <c r="AX41" s="6">
+        <f t="array" ref="AX41">AVERAGE(IF(($F$34:$F$663=AW35)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>85.949496190476182</v>
+      </c>
+      <c r="AY41" s="6"/>
+      <c r="AZ41" s="6">
+        <f t="array" ref="AZ41">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BA30)*($E$34:$E$663=BA31)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>89.775120000000015</v>
+      </c>
+      <c r="BA41" s="6"/>
+      <c r="BB41" s="6">
+        <f t="array" ref="BB41">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>87.20999333333333</v>
+      </c>
+      <c r="BC41" s="6"/>
+      <c r="BD41" s="6">
+        <f t="array" ref="BD41">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>85.240666666666655</v>
+      </c>
+      <c r="BE41" s="6"/>
+      <c r="BF41" s="6">
+        <f t="array" ref="BF41">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>81.958826666666667</v>
+      </c>
+      <c r="BG41" s="6"/>
+      <c r="BH41" s="6">
+        <f t="array" ref="BH41">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>88.014206666666681</v>
+      </c>
+      <c r="BI41" s="6"/>
+      <c r="BJ41" s="6">
+        <f t="array" ref="BJ41">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>86.138979999999989</v>
+      </c>
+      <c r="BK41" s="6"/>
+      <c r="BL41" s="6">
+        <f t="array" ref="BL41">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($G$34:$G$663=AW41),$I$34:$I$663))</f>
+        <v>83.308680000000024</v>
+      </c>
+      <c r="BM41" s="6"/>
+      <c r="BO41">
+        <v>20</v>
+      </c>
+      <c r="BP41" s="6">
+        <f t="array" ref="BP41">AVERAGE(IF(($F$34:$F$663=BO35)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>85.641422857142842</v>
+      </c>
+      <c r="BQ41" s="6"/>
+      <c r="BR41" s="6">
+        <f t="array" ref="BR41">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BS30)*($E$34:$E$663=BS31)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>85.926446666666664</v>
+      </c>
+      <c r="BS41" s="6"/>
+      <c r="BT41" s="6">
+        <f t="array" ref="BT41">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>87.55398666666666</v>
+      </c>
+      <c r="BU41" s="6"/>
+      <c r="BV41" s="6">
+        <f t="array" ref="BV41">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>86.176086666666649</v>
+      </c>
+      <c r="BW41" s="6"/>
+      <c r="BX41" s="6">
+        <f t="array" ref="BX41">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>81.161293333333333</v>
+      </c>
+      <c r="BY41" s="6"/>
+      <c r="BZ41" s="6">
+        <f t="array" ref="BZ41">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>87.62103333333333</v>
+      </c>
+      <c r="CA41" s="6"/>
+      <c r="CB41" s="6">
+        <f t="array" ref="CB41">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>87.089320000000015</v>
+      </c>
+      <c r="CC41" s="6"/>
+      <c r="CD41" s="6">
+        <f t="array" ref="CD41">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($G$34:$G$663=BO41),$J$34:$J$663))</f>
+        <v>83.961793333333347</v>
+      </c>
+      <c r="CE41" s="6"/>
+    </row>
+    <row r="42" spans="3:83">
       <c r="C42">
         <v>2E-3</v>
       </c>
@@ -2838,8 +4222,40 @@
       <c r="AU42" s="6">
         <v>83.855043198213409</v>
       </c>
-    </row>
-    <row r="43" spans="3:47">
+      <c r="AX42" s="6"/>
+      <c r="AY42" s="6"/>
+      <c r="AZ42" s="6"/>
+      <c r="BA42" s="6"/>
+      <c r="BB42" s="6"/>
+      <c r="BC42" s="6"/>
+      <c r="BD42" s="6"/>
+      <c r="BE42" s="6"/>
+      <c r="BF42" s="6"/>
+      <c r="BG42" s="6"/>
+      <c r="BH42" s="6"/>
+      <c r="BI42" s="6"/>
+      <c r="BJ42" s="6"/>
+      <c r="BK42" s="6"/>
+      <c r="BL42" s="6"/>
+      <c r="BM42" s="6"/>
+      <c r="BP42" s="6"/>
+      <c r="BQ42" s="6"/>
+      <c r="BR42" s="6"/>
+      <c r="BS42" s="6"/>
+      <c r="BT42" s="6"/>
+      <c r="BU42" s="6"/>
+      <c r="BV42" s="6"/>
+      <c r="BW42" s="6"/>
+      <c r="BX42" s="6"/>
+      <c r="BY42" s="6"/>
+      <c r="BZ42" s="6"/>
+      <c r="CA42" s="6"/>
+      <c r="CB42" s="6"/>
+      <c r="CC42" s="6"/>
+      <c r="CD42" s="6"/>
+      <c r="CE42" s="6"/>
+    </row>
+    <row r="43" spans="3:83">
       <c r="C43">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -2912,8 +4328,40 @@
       <c r="AU43" s="6">
         <v>84.684906295635955</v>
       </c>
-    </row>
-    <row r="44" spans="3:47">
+      <c r="AX43" s="6"/>
+      <c r="AY43" s="6"/>
+      <c r="AZ43" s="6"/>
+      <c r="BA43" s="6"/>
+      <c r="BB43" s="6"/>
+      <c r="BC43" s="6"/>
+      <c r="BD43" s="6"/>
+      <c r="BE43" s="6"/>
+      <c r="BF43" s="6"/>
+      <c r="BG43" s="6"/>
+      <c r="BH43" s="6"/>
+      <c r="BI43" s="6"/>
+      <c r="BJ43" s="6"/>
+      <c r="BK43" s="6"/>
+      <c r="BL43" s="6"/>
+      <c r="BM43" s="6"/>
+      <c r="BP43" s="6"/>
+      <c r="BQ43" s="6"/>
+      <c r="BR43" s="6"/>
+      <c r="BS43" s="6"/>
+      <c r="BT43" s="6"/>
+      <c r="BU43" s="6"/>
+      <c r="BV43" s="6"/>
+      <c r="BW43" s="6"/>
+      <c r="BX43" s="6"/>
+      <c r="BY43" s="6"/>
+      <c r="BZ43" s="6"/>
+      <c r="CA43" s="6"/>
+      <c r="CB43" s="6"/>
+      <c r="CC43" s="6"/>
+      <c r="CD43" s="6"/>
+      <c r="CE43" s="6"/>
+    </row>
+    <row r="44" spans="3:83">
       <c r="C44">
         <v>0</v>
       </c>
@@ -2989,8 +4437,46 @@
       <c r="AU44" s="6">
         <v>85.429122877256646</v>
       </c>
-    </row>
-    <row r="45" spans="3:47">
+      <c r="AW44" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX44" s="6"/>
+      <c r="AY44" s="6"/>
+      <c r="AZ44" s="6"/>
+      <c r="BA44" s="6"/>
+      <c r="BB44" s="6"/>
+      <c r="BC44" s="6"/>
+      <c r="BD44" s="6"/>
+      <c r="BE44" s="6"/>
+      <c r="BF44" s="6"/>
+      <c r="BG44" s="6"/>
+      <c r="BH44" s="6"/>
+      <c r="BI44" s="6"/>
+      <c r="BJ44" s="6"/>
+      <c r="BK44" s="6"/>
+      <c r="BL44" s="6"/>
+      <c r="BM44" s="6"/>
+      <c r="BO44" t="s">
+        <v>59</v>
+      </c>
+      <c r="BP44" s="6"/>
+      <c r="BQ44" s="6"/>
+      <c r="BR44" s="6"/>
+      <c r="BS44" s="6"/>
+      <c r="BT44" s="6"/>
+      <c r="BU44" s="6"/>
+      <c r="BV44" s="6"/>
+      <c r="BW44" s="6"/>
+      <c r="BX44" s="6"/>
+      <c r="BY44" s="6"/>
+      <c r="BZ44" s="6"/>
+      <c r="CA44" s="6"/>
+      <c r="CB44" s="6"/>
+      <c r="CC44" s="6"/>
+      <c r="CD44" s="6"/>
+      <c r="CE44" s="6"/>
+    </row>
+    <row r="45" spans="3:83">
       <c r="C45">
         <v>5.0000000000000001E-4</v>
       </c>
@@ -3093,8 +4579,94 @@
       <c r="AN45" s="6"/>
       <c r="AO45" s="6"/>
       <c r="AP45" s="6"/>
-    </row>
-    <row r="46" spans="3:47">
+      <c r="AW45">
+        <v>35</v>
+      </c>
+      <c r="AX45" s="6">
+        <f t="array" ref="AX45">AVERAGE(IF(($F$34:$F$663=AW35)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>87.438878095238081</v>
+      </c>
+      <c r="AY45" s="6"/>
+      <c r="AZ45" s="6">
+        <f t="array" ref="AZ45">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BA30)*($E$34:$E$663=BA31)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>90.945119999999989</v>
+      </c>
+      <c r="BA45" s="6"/>
+      <c r="BB45" s="6">
+        <f t="array" ref="BB45">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>88.65506000000002</v>
+      </c>
+      <c r="BC45" s="6"/>
+      <c r="BD45" s="6">
+        <f t="array" ref="BD45">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>86.783519999999996</v>
+      </c>
+      <c r="BE45" s="6"/>
+      <c r="BF45" s="6">
+        <f t="array" ref="BF45">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>83.67397333333335</v>
+      </c>
+      <c r="BG45" s="6"/>
+      <c r="BH45" s="6">
+        <f t="array" ref="BH45">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>89.388080000000002</v>
+      </c>
+      <c r="BI45" s="6"/>
+      <c r="BJ45" s="6">
+        <f t="array" ref="BJ45">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>87.648973333333331</v>
+      </c>
+      <c r="BK45" s="6"/>
+      <c r="BL45" s="6">
+        <f t="array" ref="BL45">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($H$34:$H$663=AW45),$I$34:$I$663))</f>
+        <v>84.977419999999981</v>
+      </c>
+      <c r="BM45" s="6"/>
+      <c r="BO45">
+        <v>35</v>
+      </c>
+      <c r="BP45" s="6">
+        <f t="array" ref="BP45">AVERAGE(IF(($F$34:$F$663=BO35)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>82.379989523809513</v>
+      </c>
+      <c r="BQ45" s="6"/>
+      <c r="BR45" s="6">
+        <f t="array" ref="BR45">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BS30)*($E$34:$E$663=BS31)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>81.609380000000002</v>
+      </c>
+      <c r="BS45" s="6"/>
+      <c r="BT45" s="6">
+        <f t="array" ref="BT45">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>84.340206666666674</v>
+      </c>
+      <c r="BU45" s="6"/>
+      <c r="BV45" s="6">
+        <f t="array" ref="BV45">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>83.510613333333339</v>
+      </c>
+      <c r="BW45" s="6"/>
+      <c r="BX45" s="6">
+        <f t="array" ref="BX45">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>77.69913333333335</v>
+      </c>
+      <c r="BY45" s="6"/>
+      <c r="BZ45" s="6">
+        <f t="array" ref="BZ45">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>83.968979999999974</v>
+      </c>
+      <c r="CA45" s="6"/>
+      <c r="CB45" s="6">
+        <f t="array" ref="CB45">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>84.253266666666661</v>
+      </c>
+      <c r="CC45" s="6"/>
+      <c r="CD45" s="6">
+        <f t="array" ref="CD45">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($H$34:$H$663=BO45),$J$34:$J$663))</f>
+        <v>81.278346666666692</v>
+      </c>
+      <c r="CE45" s="6"/>
+    </row>
+    <row r="46" spans="3:83">
       <c r="C46">
         <v>1E-3</v>
       </c>
@@ -3200,8 +4772,94 @@
       <c r="AN46" s="6"/>
       <c r="AO46" s="6"/>
       <c r="AP46" s="6"/>
-    </row>
-    <row r="47" spans="3:47">
+      <c r="AW46">
+        <v>45</v>
+      </c>
+      <c r="AX46" s="6">
+        <f t="array" ref="AX46">AVERAGE(IF(($F$34:$F$663=AW35)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>86.926986666666664</v>
+      </c>
+      <c r="AY46" s="6"/>
+      <c r="AZ46" s="6">
+        <f t="array" ref="AZ46">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BA30)*($E$34:$E$663=BA31)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>90.551246666666671</v>
+      </c>
+      <c r="BA46" s="6"/>
+      <c r="BB46" s="6">
+        <f t="array" ref="BB46">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>88.154046666666673</v>
+      </c>
+      <c r="BC46" s="6"/>
+      <c r="BD46" s="6">
+        <f t="array" ref="BD46">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>86.248826666666687</v>
+      </c>
+      <c r="BE46" s="6"/>
+      <c r="BF46" s="6">
+        <f t="array" ref="BF46">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>83.097253333333342</v>
+      </c>
+      <c r="BG46" s="6"/>
+      <c r="BH46" s="6">
+        <f t="array" ref="BH46">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>88.91467333333334</v>
+      </c>
+      <c r="BI46" s="6"/>
+      <c r="BJ46" s="6">
+        <f t="array" ref="BJ46">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>87.125386666666657</v>
+      </c>
+      <c r="BK46" s="6"/>
+      <c r="BL46" s="6">
+        <f t="array" ref="BL46">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($H$34:$H$663=AW46),$I$34:$I$663))</f>
+        <v>84.397473333333338</v>
+      </c>
+      <c r="BM46" s="6"/>
+      <c r="BO46">
+        <v>45</v>
+      </c>
+      <c r="BP46" s="6">
+        <f t="array" ref="BP46">AVERAGE(IF(($F$34:$F$663=BO35)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>85.348445714285717</v>
+      </c>
+      <c r="BQ46" s="6"/>
+      <c r="BR46" s="6">
+        <f t="array" ref="BR46">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BS30)*($E$34:$E$663=BS31)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>85.229193333333342</v>
+      </c>
+      <c r="BS46" s="6"/>
+      <c r="BT46" s="6">
+        <f t="array" ref="BT46">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>87.43874000000001</v>
+      </c>
+      <c r="BU46" s="6"/>
+      <c r="BV46" s="6">
+        <f t="array" ref="BV46">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>86.088379999999987</v>
+      </c>
+      <c r="BW46" s="6"/>
+      <c r="BX46" s="6">
+        <f t="array" ref="BX46">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>80.589506666666665</v>
+      </c>
+      <c r="BY46" s="6"/>
+      <c r="BZ46" s="6">
+        <f t="array" ref="BZ46">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>87.395320000000012</v>
+      </c>
+      <c r="CA46" s="6"/>
+      <c r="CB46" s="6">
+        <f t="array" ref="CB46">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>86.997553333333343</v>
+      </c>
+      <c r="CC46" s="6"/>
+      <c r="CD46" s="6">
+        <f t="array" ref="CD46">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($H$34:$H$663=BO46),$J$34:$J$663))</f>
+        <v>83.700426666666672</v>
+      </c>
+      <c r="CE46" s="6"/>
+    </row>
+    <row r="47" spans="3:83">
       <c r="C47">
         <v>2E-3</v>
       </c>
@@ -3304,8 +4962,94 @@
       <c r="AN47" s="6"/>
       <c r="AO47" s="6"/>
       <c r="AP47" s="6"/>
-    </row>
-    <row r="48" spans="3:47">
+      <c r="AW47">
+        <v>60</v>
+      </c>
+      <c r="AX47" s="6">
+        <f t="array" ref="AX47">AVERAGE(IF(($F$34:$F$663=AW35)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>86.015236190476159</v>
+      </c>
+      <c r="AY47" s="6"/>
+      <c r="AZ47" s="6">
+        <f t="array" ref="AZ47">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BA30)*($E$34:$E$663=BA31)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>89.875313333333324</v>
+      </c>
+      <c r="BA47" s="6"/>
+      <c r="BB47" s="6">
+        <f t="array" ref="BB47">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BC30)*($E$34:$E$663=BC31)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>87.277153333333345</v>
+      </c>
+      <c r="BC47" s="6"/>
+      <c r="BD47" s="6">
+        <f t="array" ref="BD47">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BE30)*($E$34:$E$663=BE31)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>85.274453333333341</v>
+      </c>
+      <c r="BE47" s="6"/>
+      <c r="BF47" s="6">
+        <f t="array" ref="BF47">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BG30)*($E$34:$E$663=BG31)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>82.025413333333347</v>
+      </c>
+      <c r="BG47" s="6"/>
+      <c r="BH47" s="6">
+        <f t="array" ref="BH47">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BI30)*($E$34:$E$663=BI31)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>88.086380000000005</v>
+      </c>
+      <c r="BI47" s="6"/>
+      <c r="BJ47" s="6">
+        <f t="array" ref="BJ47">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BK30)*($E$34:$E$663=BK31)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>86.191559999999996</v>
+      </c>
+      <c r="BK47" s="6"/>
+      <c r="BL47" s="6">
+        <f t="array" ref="BL47">AVERAGE(IF(($F$34:$F$663=AW35)*($D$34:$D$663=BM30)*($E$34:$E$663=BM31)*($H$34:$H$663=AW47),$I$34:$I$663))</f>
+        <v>83.376379999999997</v>
+      </c>
+      <c r="BM47" s="6"/>
+      <c r="BO47">
+        <v>60</v>
+      </c>
+      <c r="BP47" s="6">
+        <f t="array" ref="BP47">AVERAGE(IF(($F$34:$F$663=BO35)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>87.997920000000008</v>
+      </c>
+      <c r="BQ47" s="6"/>
+      <c r="BR47" s="6">
+        <f t="array" ref="BR47">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BS30)*($E$34:$E$663=BS31)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>88.219700000000003</v>
+      </c>
+      <c r="BS47" s="6"/>
+      <c r="BT47" s="6">
+        <f t="array" ref="BT47">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BU30)*($E$34:$E$663=BU31)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>89.866586666666677</v>
+      </c>
+      <c r="BU47" s="6"/>
+      <c r="BV47" s="6">
+        <f t="array" ref="BV47">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BW30)*($E$34:$E$663=BW31)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>88.448746666666651</v>
+      </c>
+      <c r="BW47" s="6"/>
+      <c r="BX47" s="6">
+        <f t="array" ref="BX47">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=BY30)*($E$34:$E$663=BY31)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>83.762540000000001</v>
+      </c>
+      <c r="BY47" s="6"/>
+      <c r="BZ47" s="6">
+        <f t="array" ref="BZ47">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CA30)*($E$34:$E$663=CA31)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>90.005593333333323</v>
+      </c>
+      <c r="CA47" s="6"/>
+      <c r="CB47" s="6">
+        <f t="array" ref="CB47">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CC30)*($E$34:$E$663=CC31)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>89.350313333333332</v>
+      </c>
+      <c r="CC47" s="6"/>
+      <c r="CD47" s="6">
+        <f t="array" ref="CD47">AVERAGE(IF(($F$34:$F$663=BO35)*($D$34:$D$663=CE30)*($E$34:$E$663=CE31)*($H$34:$H$663=BO47),$J$34:$J$663))</f>
+        <v>86.331960000000009</v>
+      </c>
+      <c r="CE47" s="6"/>
+    </row>
+    <row r="48" spans="3:83">
       <c r="C48">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -24446,11 +26190,11 @@
         <v>86.652799999999999</v>
       </c>
       <c r="K610">
-        <f t="shared" ref="K610:K673" si="18">2*I610*J610/(I610+J610)</f>
+        <f t="shared" ref="K610:K663" si="18">2*I610*J610/(I610+J610)</f>
         <v>83.870865862925712</v>
       </c>
       <c r="L610" t="str">
-        <f t="shared" ref="L610:L673" si="19">IF(MOD(ROW(K610), 5)=4,AVERAGE(K610:K614),"")</f>
+        <f t="shared" ref="L610:L663" si="19">IF(MOD(ROW(K610), 5)=4,AVERAGE(K610:K614),"")</f>
         <v/>
       </c>
     </row>
@@ -26414,8 +28158,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="BM13" r:id="rId1"/>
+    <hyperlink ref="BM14" r:id="rId2"/>
+    <hyperlink ref="BM15:BM24" r:id="rId3" display="\\"/>
+  </hyperlinks>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.0629921259842521" bottom="1.0629921259842521" header="0.78740157480314965" footer="0.78740157480314965"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -26423,7 +28172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:CH124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BC92" sqref="BC92"/>
     </sheetView>
   </sheetViews>
@@ -26751,7 +28500,7 @@
         <v>2.2129400000000001</v>
       </c>
       <c r="AF5">
-        <f>(2*$Y5+1)*(2*$Y5+1)/($Z5*$AA5)</f>
+        <f t="shared" ref="AF5:AF36" si="0">(2*$Y5+1)*(2*$Y5+1)/($Z5*$AA5)</f>
         <v>6.25</v>
       </c>
       <c r="AI5">
@@ -26779,7 +28528,7 @@
         <v>4.2717499999999999</v>
       </c>
       <c r="AQ5">
-        <f>(2*$AJ5+1)*(2*$AJ5+1)/($AK5*$AL5)</f>
+        <f t="shared" ref="AQ5:AQ36" si="1">(2*$AJ5+1)*(2*$AJ5+1)/($AK5*$AL5)</f>
         <v>6.25</v>
       </c>
       <c r="AT5">
@@ -26965,7 +28714,7 @@
         <v>2.2304900000000001</v>
       </c>
       <c r="AF6">
-        <f>(2*$Y6+1)*(2*$Y6+1)/($Z6*$AA6)</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="AI6">
@@ -26993,7 +28742,7 @@
         <v>4.2107200000000002</v>
       </c>
       <c r="AQ6">
-        <f>(2*$AJ6+1)*(2*$AJ6+1)/($AK6*$AL6)</f>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="AT6">
@@ -27179,7 +28928,7 @@
         <v>2.2048999999999999</v>
       </c>
       <c r="AF7">
-        <f>(2*$Y7+1)*(2*$Y7+1)/($Z7*$AA7)</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="AI7">
@@ -27207,7 +28956,7 @@
         <v>4.1601800000000004</v>
       </c>
       <c r="AQ7">
-        <f>(2*$AJ7+1)*(2*$AJ7+1)/($AK7*$AL7)</f>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="AT7">
@@ -27393,7 +29142,7 @@
         <v>2.3817900000000001</v>
       </c>
       <c r="AF8">
-        <f>(2*$Y8+1)*(2*$Y8+1)/($Z8*$AA8)</f>
+        <f t="shared" si="0"/>
         <v>20.25</v>
       </c>
       <c r="AI8">
@@ -27421,7 +29170,7 @@
         <v>4.7919299999999998</v>
       </c>
       <c r="AQ8">
-        <f>(2*$AJ8+1)*(2*$AJ8+1)/($AK8*$AL8)</f>
+        <f t="shared" si="1"/>
         <v>20.25</v>
       </c>
       <c r="AR8" t="s">
@@ -27610,7 +29359,7 @@
         <v>2.1253000000000002</v>
       </c>
       <c r="AF9">
-        <f>(2*$Y9+1)*(2*$Y9+1)/($Z9*$AA9)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="AI9">
@@ -27638,7 +29387,7 @@
         <v>4.0585699999999996</v>
       </c>
       <c r="AQ9">
-        <f>(2*$AJ9+1)*(2*$AJ9+1)/($AK9*$AL9)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="AT9">
@@ -27824,7 +29573,7 @@
         <v>2.37514</v>
       </c>
       <c r="AF10">
-        <f>(2*$Y10+1)*(2*$Y10+1)/($Z10*$AA10)</f>
+        <f t="shared" si="0"/>
         <v>40.5</v>
       </c>
       <c r="AI10">
@@ -27852,7 +29601,7 @@
         <v>4.7340099999999996</v>
       </c>
       <c r="AQ10">
-        <f>(2*$AJ10+1)*(2*$AJ10+1)/($AK10*$AL10)</f>
+        <f t="shared" si="1"/>
         <v>40.5</v>
       </c>
       <c r="AT10">
@@ -28038,7 +29787,7 @@
         <v>2.3788299999999998</v>
       </c>
       <c r="AF11">
-        <f>(2*$Y11+1)*(2*$Y11+1)/($Z11*$AA11)</f>
+        <f t="shared" si="0"/>
         <v>40.5</v>
       </c>
       <c r="AI11">
@@ -28066,7 +29815,7 @@
         <v>4.6681400000000002</v>
       </c>
       <c r="AQ11">
-        <f>(2*$AJ11+1)*(2*$AJ11+1)/($AK11*$AL11)</f>
+        <f t="shared" si="1"/>
         <v>40.5</v>
       </c>
       <c r="AT11">
@@ -28234,7 +29983,7 @@
         <v>2.4830700000000001</v>
       </c>
       <c r="AF12">
-        <f>(2*$Y12+1)*(2*$Y12+1)/($Z12*$AA12)</f>
+        <f t="shared" si="0"/>
         <v>42.25</v>
       </c>
       <c r="AI12">
@@ -28262,7 +30011,7 @@
         <v>5.2835299999999998</v>
       </c>
       <c r="AQ12">
-        <f>(2*$AJ12+1)*(2*$AJ12+1)/($AK12*$AL12)</f>
+        <f t="shared" si="1"/>
         <v>42.25</v>
       </c>
       <c r="AT12">
@@ -28433,7 +30182,7 @@
         <v>2.56393</v>
       </c>
       <c r="AF13">
-        <f>(2*$Y13+1)*(2*$Y13+1)/($Z13*$AA13)</f>
+        <f t="shared" si="0"/>
         <v>72.25</v>
       </c>
       <c r="AI13">
@@ -28461,7 +30210,7 @@
         <v>5.7723300000000002</v>
       </c>
       <c r="AQ13">
-        <f>(2*$AJ13+1)*(2*$AJ13+1)/($AK13*$AL13)</f>
+        <f t="shared" si="1"/>
         <v>72.25</v>
       </c>
       <c r="AR13" t="s">
@@ -28632,7 +30381,7 @@
         <v>2.33643</v>
       </c>
       <c r="AF14">
-        <f>(2*$Y14+1)*(2*$Y14+1)/($Z14*$AA14)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="AI14">
@@ -28660,7 +30409,7 @@
         <v>4.5893300000000004</v>
       </c>
       <c r="AQ14">
-        <f>(2*$AJ14+1)*(2*$AJ14+1)/($AK14*$AL14)</f>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="AT14">
@@ -28828,7 +30577,7 @@
         <v>2.4889100000000002</v>
       </c>
       <c r="AF15">
-        <f>(2*$Y15+1)*(2*$Y15+1)/($Z15*$AA15)</f>
+        <f t="shared" si="0"/>
         <v>84.5</v>
       </c>
       <c r="AI15">
@@ -28856,7 +30605,7 @@
         <v>5.22288</v>
       </c>
       <c r="AQ15">
-        <f>(2*$AJ15+1)*(2*$AJ15+1)/($AK15*$AL15)</f>
+        <f t="shared" si="1"/>
         <v>84.5</v>
       </c>
       <c r="AT15">
@@ -29027,7 +30776,7 @@
         <v>2.4851299999999998</v>
       </c>
       <c r="AF16">
-        <f>(2*$Y16+1)*(2*$Y16+1)/($Z16*$AA16)</f>
+        <f t="shared" si="0"/>
         <v>84.5</v>
       </c>
       <c r="AI16">
@@ -29055,7 +30804,7 @@
         <v>5.16594</v>
       </c>
       <c r="AQ16">
-        <f>(2*$AJ16+1)*(2*$AJ16+1)/($AK16*$AL16)</f>
+        <f t="shared" si="1"/>
         <v>84.5</v>
       </c>
       <c r="AT16">
@@ -29223,7 +30972,7 @@
         <v>2.57491</v>
       </c>
       <c r="AF17">
-        <f>(2*$Y17+1)*(2*$Y17+1)/($Z17*$AA17)</f>
+        <f t="shared" si="0"/>
         <v>144.5</v>
       </c>
       <c r="AI17">
@@ -29251,7 +31000,7 @@
         <v>5.7058299999999997</v>
       </c>
       <c r="AQ17">
-        <f>(2*$AJ17+1)*(2*$AJ17+1)/($AK17*$AL17)</f>
+        <f t="shared" si="1"/>
         <v>144.5</v>
       </c>
       <c r="AT17">
@@ -29419,7 +31168,7 @@
         <v>2.5695600000000001</v>
       </c>
       <c r="AF18">
-        <f>(2*$Y18+1)*(2*$Y18+1)/($Z18*$AA18)</f>
+        <f t="shared" si="0"/>
         <v>144.5</v>
       </c>
       <c r="AI18">
@@ -29447,7 +31196,7 @@
         <v>5.6483600000000003</v>
       </c>
       <c r="AQ18">
-        <f>(2*$AJ18+1)*(2*$AJ18+1)/($AK18*$AL18)</f>
+        <f t="shared" si="1"/>
         <v>144.5</v>
       </c>
       <c r="AR18" t="s">
@@ -29618,7 +31367,7 @@
         <v>2.4664000000000001</v>
       </c>
       <c r="AF19">
-        <f>(2*$Y19+1)*(2*$Y19+1)/($Z19*$AA19)</f>
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
       <c r="AI19">
@@ -29646,7 +31395,7 @@
         <v>5.0894000000000004</v>
       </c>
       <c r="AQ19">
-        <f>(2*$AJ19+1)*(2*$AJ19+1)/($AK19*$AL19)</f>
+        <f t="shared" si="1"/>
         <v>169</v>
       </c>
       <c r="AR19" t="s">
@@ -29817,7 +31566,7 @@
         <v>2.5566</v>
       </c>
       <c r="AF20">
-        <f>(2*$Y20+1)*(2*$Y20+1)/($Z20*$AA20)</f>
+        <f t="shared" si="0"/>
         <v>289</v>
       </c>
       <c r="AG20" t="s">
@@ -29848,7 +31597,7 @@
         <v>5.5700500000000002</v>
       </c>
       <c r="AQ20">
-        <f>(2*$AJ20+1)*(2*$AJ20+1)/($AK20*$AL20)</f>
+        <f t="shared" si="1"/>
         <v>289</v>
       </c>
       <c r="AT20">
@@ -30019,7 +31768,7 @@
         <v>5.3068099999999996</v>
       </c>
       <c r="AF21">
-        <f>(2*$Y21+1)*(2*$Y21+1)/($Z21*$AA21)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="AI21">
@@ -30047,7 +31796,7 @@
         <v>7.0457000000000001</v>
       </c>
       <c r="AQ21">
-        <f>(2*$AJ21+1)*(2*$AJ21+1)/($AK21*$AL21)</f>
+        <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
       <c r="AT21">
@@ -30215,7 +31964,7 @@
         <v>5.3213999999999997</v>
       </c>
       <c r="AF22">
-        <f>(2*$Y22+1)*(2*$Y22+1)/($Z22*$AA22)</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="AI22">
@@ -30243,7 +31992,7 @@
         <v>6.5672499999999996</v>
       </c>
       <c r="AQ22">
-        <f>(2*$AJ22+1)*(2*$AJ22+1)/($AK22*$AL22)</f>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="AT22">
@@ -30411,7 +32160,7 @@
         <v>4.8365400000000003</v>
       </c>
       <c r="AF23">
-        <f>(2*$Y23+1)*(2*$Y23+1)/($Z23*$AA23)</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="AI23">
@@ -30439,7 +32188,7 @@
         <v>6.97262</v>
       </c>
       <c r="AQ23">
-        <f>(2*$AJ23+1)*(2*$AJ23+1)/($AK23*$AL23)</f>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="AT23">
@@ -30607,7 +32356,7 @@
         <v>3.8314900000000001</v>
       </c>
       <c r="AF24">
-        <f>(2*$Y24+1)*(2*$Y24+1)/($Z24*$AA24)</f>
+        <f t="shared" si="0"/>
         <v>20.25</v>
       </c>
       <c r="AI24">
@@ -30635,7 +32384,7 @@
         <v>5.9458900000000003</v>
       </c>
       <c r="AQ24">
-        <f>(2*$AJ24+1)*(2*$AJ24+1)/($AK24*$AL24)</f>
+        <f t="shared" si="1"/>
         <v>20.25</v>
       </c>
       <c r="AT24">
@@ -30803,7 +32552,7 @@
         <v>4.9438800000000001</v>
       </c>
       <c r="AF25">
-        <f>(2*$Y25+1)*(2*$Y25+1)/($Z25*$AA25)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="AI25">
@@ -30831,7 +32580,7 @@
         <v>6.6167299999999996</v>
       </c>
       <c r="AQ25">
-        <f>(2*$AJ25+1)*(2*$AJ25+1)/($AK25*$AL25)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="AT25">
@@ -30999,7 +32748,7 @@
         <v>3.7054499999999999</v>
       </c>
       <c r="AF26">
-        <f>(2*$Y26+1)*(2*$Y26+1)/($Z26*$AA26)</f>
+        <f t="shared" si="0"/>
         <v>40.5</v>
       </c>
       <c r="AI26">
@@ -31027,7 +32776,7 @@
         <v>6.05288</v>
       </c>
       <c r="AQ26">
-        <f>(2*$AJ26+1)*(2*$AJ26+1)/($AK26*$AL26)</f>
+        <f t="shared" si="1"/>
         <v>40.5</v>
       </c>
       <c r="AT26">
@@ -31195,7 +32944,7 @@
         <v>3.95797</v>
       </c>
       <c r="AF27">
-        <f>(2*$Y27+1)*(2*$Y27+1)/($Z27*$AA27)</f>
+        <f t="shared" si="0"/>
         <v>40.5</v>
       </c>
       <c r="AI27">
@@ -31223,7 +32972,7 @@
         <v>5.7356699999999998</v>
       </c>
       <c r="AQ27">
-        <f>(2*$AJ27+1)*(2*$AJ27+1)/($AK27*$AL27)</f>
+        <f t="shared" si="1"/>
         <v>40.5</v>
       </c>
       <c r="AT27">
@@ -31391,7 +33140,7 @@
         <v>3.4509300000000001</v>
       </c>
       <c r="AF28">
-        <f>(2*$Y28+1)*(2*$Y28+1)/($Z28*$AA28)</f>
+        <f t="shared" si="0"/>
         <v>42.25</v>
       </c>
       <c r="AI28">
@@ -31419,7 +33168,7 @@
         <v>5.9685699999999997</v>
       </c>
       <c r="AQ28">
-        <f>(2*$AJ28+1)*(2*$AJ28+1)/($AK28*$AL28)</f>
+        <f t="shared" si="1"/>
         <v>42.25</v>
       </c>
       <c r="AT28">
@@ -31587,7 +33336,7 @@
         <v>3.3420700000000001</v>
       </c>
       <c r="AF29">
-        <f>(2*$Y29+1)*(2*$Y29+1)/($Z29*$AA29)</f>
+        <f t="shared" si="0"/>
         <v>72.25</v>
       </c>
       <c r="AI29">
@@ -31615,7 +33364,7 @@
         <v>6.2744499999999999</v>
       </c>
       <c r="AQ29">
-        <f>(2*$AJ29+1)*(2*$AJ29+1)/($AK29*$AL29)</f>
+        <f t="shared" si="1"/>
         <v>72.25</v>
       </c>
       <c r="AT29">
@@ -31783,7 +33532,7 @@
         <v>3.8994800000000001</v>
       </c>
       <c r="AF30">
-        <f>(2*$Y30+1)*(2*$Y30+1)/($Z30*$AA30)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="AI30">
@@ -31811,7 +33560,7 @@
         <v>5.9096099999999998</v>
       </c>
       <c r="AQ30">
-        <f>(2*$AJ30+1)*(2*$AJ30+1)/($AK30*$AL30)</f>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="AT30">
@@ -31982,7 +33731,7 @@
         <v>3.8280500000000002</v>
       </c>
       <c r="AF31">
-        <f>(2*$Y31+1)*(2*$Y31+1)/($Z31*$AA31)</f>
+        <f t="shared" si="0"/>
         <v>84.5</v>
       </c>
       <c r="AI31">
@@ -32010,7 +33759,7 @@
         <v>6.3053299999999997</v>
       </c>
       <c r="AQ31">
-        <f>(2*$AJ31+1)*(2*$AJ31+1)/($AK31*$AL31)</f>
+        <f t="shared" si="1"/>
         <v>84.5</v>
       </c>
       <c r="AT31">
@@ -32178,7 +33927,7 @@
         <v>3.3629199999999999</v>
       </c>
       <c r="AF32">
-        <f>(2*$Y32+1)*(2*$Y32+1)/($Z32*$AA32)</f>
+        <f t="shared" si="0"/>
         <v>84.5</v>
       </c>
       <c r="AI32">
@@ -32206,7 +33955,7 @@
         <v>5.7871499999999996</v>
       </c>
       <c r="AQ32">
-        <f>(2*$AJ32+1)*(2*$AJ32+1)/($AK32*$AL32)</f>
+        <f t="shared" si="1"/>
         <v>84.5</v>
       </c>
       <c r="AT32">
@@ -32374,7 +34123,7 @@
         <v>3.8421799999999999</v>
       </c>
       <c r="AF33">
-        <f>(2*$Y33+1)*(2*$Y33+1)/($Z33*$AA33)</f>
+        <f t="shared" si="0"/>
         <v>144.5</v>
       </c>
       <c r="AI33">
@@ -32402,7 +34151,7 @@
         <v>6.71347</v>
       </c>
       <c r="AQ33">
-        <f>(2*$AJ33+1)*(2*$AJ33+1)/($AK33*$AL33)</f>
+        <f t="shared" si="1"/>
         <v>144.5</v>
       </c>
       <c r="AT33">
@@ -32570,7 +34319,7 @@
         <v>3.28172</v>
       </c>
       <c r="AF34">
-        <f>(2*$Y34+1)*(2*$Y34+1)/($Z34*$AA34)</f>
+        <f t="shared" si="0"/>
         <v>144.5</v>
       </c>
       <c r="AI34">
@@ -32598,7 +34347,7 @@
         <v>6.1071900000000001</v>
       </c>
       <c r="AQ34">
-        <f>(2*$AJ34+1)*(2*$AJ34+1)/($AK34*$AL34)</f>
+        <f t="shared" si="1"/>
         <v>144.5</v>
       </c>
       <c r="AT34">
@@ -32766,7 +34515,7 @@
         <v>3.7867700000000002</v>
       </c>
       <c r="AF35">
-        <f>(2*$Y35+1)*(2*$Y35+1)/($Z35*$AA35)</f>
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
       <c r="AI35">
@@ -32794,7 +34543,7 @@
         <v>6.1670199999999999</v>
       </c>
       <c r="AQ35">
-        <f>(2*$AJ35+1)*(2*$AJ35+1)/($AK35*$AL35)</f>
+        <f t="shared" si="1"/>
         <v>169</v>
       </c>
       <c r="AT35">
@@ -32962,7 +34711,7 @@
         <v>3.8056299999999998</v>
       </c>
       <c r="AF36">
-        <f>(2*$Y36+1)*(2*$Y36+1)/($Z36*$AA36)</f>
+        <f t="shared" si="0"/>
         <v>289</v>
       </c>
       <c r="AI36">
@@ -32990,7 +34739,7 @@
         <v>6.5723799999999999</v>
       </c>
       <c r="AQ36">
-        <f>(2*$AJ36+1)*(2*$AJ36+1)/($AK36*$AL36)</f>
+        <f t="shared" si="1"/>
         <v>289</v>
       </c>
       <c r="AT36">
@@ -33158,7 +34907,7 @@
         <v>8.3100400000000008</v>
       </c>
       <c r="AF37">
-        <f>(2*$Y37+1)*(2*$Y37+1)/($Z37*$AA37)</f>
+        <f t="shared" ref="AF37:AF68" si="2">(2*$Y37+1)*(2*$Y37+1)/($Z37*$AA37)</f>
         <v>6.25</v>
       </c>
       <c r="AI37">
@@ -33186,7 +34935,7 @@
         <v>9.8965399999999999</v>
       </c>
       <c r="AQ37">
-        <f>(2*$AJ37+1)*(2*$AJ37+1)/($AK37*$AL37)</f>
+        <f t="shared" ref="AQ37:AQ68" si="3">(2*$AJ37+1)*(2*$AJ37+1)/($AK37*$AL37)</f>
         <v>6.25</v>
       </c>
       <c r="AT37">
@@ -33354,7 +35103,7 @@
         <v>8.3137600000000003</v>
       </c>
       <c r="AF38">
-        <f>(2*$Y38+1)*(2*$Y38+1)/($Z38*$AA38)</f>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="AI38">
@@ -33382,7 +35131,7 @@
         <v>9.2576300000000007</v>
       </c>
       <c r="AQ38">
-        <f>(2*$AJ38+1)*(2*$AJ38+1)/($AK38*$AL38)</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="AT38">
@@ -33550,7 +35299,7 @@
         <v>7.6567999999999996</v>
       </c>
       <c r="AF39">
-        <f>(2*$Y39+1)*(2*$Y39+1)/($Z39*$AA39)</f>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="AI39">
@@ -33578,7 +35327,7 @@
         <v>9.8406099999999999</v>
       </c>
       <c r="AQ39">
-        <f>(2*$AJ39+1)*(2*$AJ39+1)/($AK39*$AL39)</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="AT39">
@@ -33746,7 +35495,7 @@
         <v>5.3140200000000002</v>
       </c>
       <c r="AF40">
-        <f>(2*$Y40+1)*(2*$Y40+1)/($Z40*$AA40)</f>
+        <f t="shared" si="2"/>
         <v>20.25</v>
       </c>
       <c r="AI40">
@@ -33774,7 +35523,7 @@
         <v>7.3088699999999998</v>
       </c>
       <c r="AQ40">
-        <f>(2*$AJ40+1)*(2*$AJ40+1)/($AK40*$AL40)</f>
+        <f t="shared" si="3"/>
         <v>20.25</v>
       </c>
       <c r="AT40">
@@ -33942,7 +35691,7 @@
         <v>7.8759399999999999</v>
       </c>
       <c r="AF41">
-        <f>(2*$Y41+1)*(2*$Y41+1)/($Z41*$AA41)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="AI41">
@@ -33970,7 +35719,7 @@
         <v>9.4288399999999992</v>
       </c>
       <c r="AQ41">
-        <f>(2*$AJ41+1)*(2*$AJ41+1)/($AK41*$AL41)</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="AT41">
@@ -34138,7 +35887,7 @@
         <v>5.1061899999999998</v>
       </c>
       <c r="AF42">
-        <f>(2*$Y42+1)*(2*$Y42+1)/($Z42*$AA42)</f>
+        <f t="shared" si="2"/>
         <v>40.5</v>
       </c>
       <c r="AI42">
@@ -34166,7 +35915,7 @@
         <v>7.88049</v>
       </c>
       <c r="AQ42">
-        <f>(2*$AJ42+1)*(2*$AJ42+1)/($AK42*$AL42)</f>
+        <f t="shared" si="3"/>
         <v>40.5</v>
       </c>
       <c r="AT42">
@@ -34334,7 +36083,7 @@
         <v>5.8903999999999996</v>
       </c>
       <c r="AF43">
-        <f>(2*$Y43+1)*(2*$Y43+1)/($Z43*$AA43)</f>
+        <f t="shared" si="2"/>
         <v>40.5</v>
       </c>
       <c r="AI43">
@@ -34362,7 +36111,7 @@
         <v>7.03721</v>
       </c>
       <c r="AQ43">
-        <f>(2*$AJ43+1)*(2*$AJ43+1)/($AK43*$AL43)</f>
+        <f t="shared" si="3"/>
         <v>40.5</v>
       </c>
       <c r="AT43">
@@ -34530,7 +36279,7 @@
         <v>4.5121700000000002</v>
       </c>
       <c r="AF44">
-        <f>(2*$Y44+1)*(2*$Y44+1)/($Z44*$AA44)</f>
+        <f t="shared" si="2"/>
         <v>42.25</v>
       </c>
       <c r="AI44">
@@ -34558,7 +36307,7 @@
         <v>6.92638</v>
       </c>
       <c r="AQ44">
-        <f>(2*$AJ44+1)*(2*$AJ44+1)/($AK44*$AL44)</f>
+        <f t="shared" si="3"/>
         <v>42.25</v>
       </c>
       <c r="AT44">
@@ -34726,7 +36475,7 @@
         <v>4.2621099999999998</v>
       </c>
       <c r="AF45">
-        <f>(2*$Y45+1)*(2*$Y45+1)/($Z45*$AA45)</f>
+        <f t="shared" si="2"/>
         <v>72.25</v>
       </c>
       <c r="AI45">
@@ -34754,7 +36503,7 @@
         <v>7.0984499999999997</v>
       </c>
       <c r="AQ45">
-        <f>(2*$AJ45+1)*(2*$AJ45+1)/($AK45*$AL45)</f>
+        <f t="shared" si="3"/>
         <v>72.25</v>
       </c>
       <c r="AT45">
@@ -34904,7 +36653,7 @@
         <v>5.8211000000000004</v>
       </c>
       <c r="AF46">
-        <f>(2*$Y46+1)*(2*$Y46+1)/($Z46*$AA46)</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="AI46">
@@ -34932,7 +36681,7 @@
         <v>7.7378</v>
       </c>
       <c r="AQ46">
-        <f>(2*$AJ46+1)*(2*$AJ46+1)/($AK46*$AL46)</f>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="AT46">
@@ -35082,7 +36831,7 @@
         <v>5.5438200000000002</v>
       </c>
       <c r="AF47">
-        <f>(2*$Y47+1)*(2*$Y47+1)/($Z47*$AA47)</f>
+        <f t="shared" si="2"/>
         <v>84.5</v>
       </c>
       <c r="AI47">
@@ -35110,7 +36859,7 @@
         <v>7.9202000000000004</v>
       </c>
       <c r="AQ47">
-        <f>(2*$AJ47+1)*(2*$AJ47+1)/($AK47*$AL47)</f>
+        <f t="shared" si="3"/>
         <v>84.5</v>
       </c>
       <c r="AT47">
@@ -35260,7 +37009,7 @@
         <v>4.3767300000000002</v>
       </c>
       <c r="AF48">
-        <f>(2*$Y48+1)*(2*$Y48+1)/($Z48*$AA48)</f>
+        <f t="shared" si="2"/>
         <v>84.5</v>
       </c>
       <c r="AI48">
@@ -35288,7 +37037,7 @@
         <v>6.7133599999999998</v>
       </c>
       <c r="AQ48">
-        <f>(2*$AJ48+1)*(2*$AJ48+1)/($AK48*$AL48)</f>
+        <f t="shared" si="3"/>
         <v>84.5</v>
       </c>
       <c r="AT48">
@@ -35438,7 +37187,7 @@
         <v>5.4931000000000001</v>
       </c>
       <c r="AF49">
-        <f>(2*$Y49+1)*(2*$Y49+1)/($Z49*$AA49)</f>
+        <f t="shared" si="2"/>
         <v>144.5</v>
       </c>
       <c r="AI49">
@@ -35466,7 +37215,7 @@
         <v>8.2604500000000005</v>
       </c>
       <c r="AQ49">
-        <f>(2*$AJ49+1)*(2*$AJ49+1)/($AK49*$AL49)</f>
+        <f t="shared" si="3"/>
         <v>144.5</v>
       </c>
       <c r="AT49">
@@ -35580,7 +37329,7 @@
         <v>4.1714099999999998</v>
       </c>
       <c r="AF50">
-        <f>(2*$Y50+1)*(2*$Y50+1)/($Z50*$AA50)</f>
+        <f t="shared" si="2"/>
         <v>144.5</v>
       </c>
       <c r="AI50">
@@ -35608,7 +37357,7 @@
         <v>6.9145799999999999</v>
       </c>
       <c r="AQ50">
-        <f>(2*$AJ50+1)*(2*$AJ50+1)/($AK50*$AL50)</f>
+        <f t="shared" si="3"/>
         <v>144.5</v>
       </c>
       <c r="AT50">
@@ -35728,7 +37477,7 @@
         <v>5.4900799999999998</v>
       </c>
       <c r="AF51">
-        <f>(2*$Y51+1)*(2*$Y51+1)/($Z51*$AA51)</f>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="AG51" t="s">
@@ -35759,7 +37508,7 @@
         <v>7.78</v>
       </c>
       <c r="AQ51">
-        <f>(2*$AJ51+1)*(2*$AJ51+1)/($AK51*$AL51)</f>
+        <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="AT51">
@@ -35873,7 +37622,7 @@
         <v>5.4398200000000001</v>
       </c>
       <c r="AF52">
-        <f>(2*$Y52+1)*(2*$Y52+1)/($Z52*$AA52)</f>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
       <c r="AI52">
@@ -35901,7 +37650,7 @@
         <v>8.1125000000000007</v>
       </c>
       <c r="AQ52">
-        <f>(2*$AJ52+1)*(2*$AJ52+1)/($AK52*$AL52)</f>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="AT52">
@@ -36015,7 +37764,7 @@
         <v>13.9656</v>
       </c>
       <c r="AF53">
-        <f>(2*$Y53+1)*(2*$Y53+1)/($Z53*$AA53)</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="AI53">
@@ -36043,7 +37792,7 @@
         <v>15.2745</v>
       </c>
       <c r="AQ53">
-        <f>(2*$AJ53+1)*(2*$AJ53+1)/($AK53*$AL53)</f>
+        <f t="shared" si="3"/>
         <v>6.25</v>
       </c>
       <c r="AT53">
@@ -36157,7 +37906,7 @@
         <v>13.796799999999999</v>
       </c>
       <c r="AF54">
-        <f>(2*$Y54+1)*(2*$Y54+1)/($Z54*$AA54)</f>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="AI54">
@@ -36185,7 +37934,7 @@
         <v>14.128500000000001</v>
       </c>
       <c r="AQ54">
-        <f>(2*$AJ54+1)*(2*$AJ54+1)/($AK54*$AL54)</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="AT54">
@@ -36299,7 +38048,7 @@
         <v>12.7704</v>
       </c>
       <c r="AF55">
-        <f>(2*$Y55+1)*(2*$Y55+1)/($Z55*$AA55)</f>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="AI55">
@@ -36327,7 +38076,7 @@
         <v>15.0854</v>
       </c>
       <c r="AQ55">
-        <f>(2*$AJ55+1)*(2*$AJ55+1)/($AK55*$AL55)</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="AT55">
@@ -36441,7 +38190,7 @@
         <v>8.3748900000000006</v>
       </c>
       <c r="AF56">
-        <f>(2*$Y56+1)*(2*$Y56+1)/($Z56*$AA56)</f>
+        <f t="shared" si="2"/>
         <v>20.25</v>
       </c>
       <c r="AI56">
@@ -36469,7 +38218,7 @@
         <v>10.129899999999999</v>
       </c>
       <c r="AQ56">
-        <f>(2*$AJ56+1)*(2*$AJ56+1)/($AK56*$AL56)</f>
+        <f t="shared" si="3"/>
         <v>20.25</v>
       </c>
       <c r="AT56">
@@ -36583,7 +38332,7 @@
         <v>12.929</v>
       </c>
       <c r="AF57">
-        <f>(2*$Y57+1)*(2*$Y57+1)/($Z57*$AA57)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="AI57">
@@ -36611,7 +38360,7 @@
         <v>14.264099999999999</v>
       </c>
       <c r="AQ57">
-        <f>(2*$AJ57+1)*(2*$AJ57+1)/($AK57*$AL57)</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="AT57">
@@ -36725,7 +38474,7 @@
         <v>7.9732500000000002</v>
       </c>
       <c r="AF58">
-        <f>(2*$Y58+1)*(2*$Y58+1)/($Z58*$AA58)</f>
+        <f t="shared" si="2"/>
         <v>40.5</v>
       </c>
       <c r="AI58">
@@ -36753,7 +38502,7 @@
         <v>10.9498</v>
       </c>
       <c r="AQ58">
-        <f>(2*$AJ58+1)*(2*$AJ58+1)/($AK58*$AL58)</f>
+        <f t="shared" si="3"/>
         <v>40.5</v>
       </c>
       <c r="AT58">
@@ -36867,7 +38616,7 @@
         <v>9.1700599999999994</v>
       </c>
       <c r="AF59">
-        <f>(2*$Y59+1)*(2*$Y59+1)/($Z59*$AA59)</f>
+        <f t="shared" si="2"/>
         <v>40.5</v>
       </c>
       <c r="AI59">
@@ -36895,7 +38644,7 @@
         <v>9.6981000000000002</v>
       </c>
       <c r="AQ59">
-        <f>(2*$AJ59+1)*(2*$AJ59+1)/($AK59*$AL59)</f>
+        <f t="shared" si="3"/>
         <v>40.5</v>
       </c>
       <c r="AT59">
@@ -37009,7 +38758,7 @@
         <v>6.8455199999999996</v>
       </c>
       <c r="AF60">
-        <f>(2*$Y60+1)*(2*$Y60+1)/($Z60*$AA60)</f>
+        <f t="shared" si="2"/>
         <v>42.25</v>
       </c>
       <c r="AI60">
@@ -37037,7 +38786,7 @@
         <v>9.0389099999999996</v>
       </c>
       <c r="AQ60">
-        <f>(2*$AJ60+1)*(2*$AJ60+1)/($AK60*$AL60)</f>
+        <f t="shared" si="3"/>
         <v>42.25</v>
       </c>
       <c r="AT60">
@@ -37157,7 +38906,7 @@
         <v>6.3443399999999999</v>
       </c>
       <c r="AF61">
-        <f>(2*$Y61+1)*(2*$Y61+1)/($Z61*$AA61)</f>
+        <f t="shared" si="2"/>
         <v>72.25</v>
       </c>
       <c r="AI61">
@@ -37185,7 +38934,7 @@
         <v>8.9656800000000008</v>
       </c>
       <c r="AQ61">
-        <f>(2*$AJ61+1)*(2*$AJ61+1)/($AK61*$AL61)</f>
+        <f t="shared" si="3"/>
         <v>72.25</v>
       </c>
       <c r="AT61">
@@ -37299,7 +39048,7 @@
         <v>8.9617799999999992</v>
       </c>
       <c r="AF62">
-        <f>(2*$Y62+1)*(2*$Y62+1)/($Z62*$AA62)</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="AI62">
@@ -37327,7 +39076,7 @@
         <v>10.694000000000001</v>
       </c>
       <c r="AQ62">
-        <f>(2*$AJ62+1)*(2*$AJ62+1)/($AK62*$AL62)</f>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="AT62">
@@ -37441,7 +39190,7 @@
         <v>8.3255999999999997</v>
       </c>
       <c r="AF63">
-        <f>(2*$Y63+1)*(2*$Y63+1)/($Z63*$AA63)</f>
+        <f t="shared" si="2"/>
         <v>84.5</v>
       </c>
       <c r="AI63">
@@ -37469,7 +39218,7 @@
         <v>10.497299999999999</v>
       </c>
       <c r="AQ63">
-        <f>(2*$AJ63+1)*(2*$AJ63+1)/($AK63*$AL63)</f>
+        <f t="shared" si="3"/>
         <v>84.5</v>
       </c>
       <c r="AT63">
@@ -37583,7 +39332,7 @@
         <v>6.5978300000000001</v>
       </c>
       <c r="AF64">
-        <f>(2*$Y64+1)*(2*$Y64+1)/($Z64*$AA64)</f>
+        <f t="shared" si="2"/>
         <v>84.5</v>
       </c>
       <c r="AI64">
@@ -37611,7 +39360,7 @@
         <v>8.74099</v>
       </c>
       <c r="AQ64">
-        <f>(2*$AJ64+1)*(2*$AJ64+1)/($AK64*$AL64)</f>
+        <f t="shared" si="3"/>
         <v>84.5</v>
       </c>
       <c r="AT64">
@@ -37725,7 +39474,7 @@
         <v>8.1184499999999993</v>
       </c>
       <c r="AF65">
-        <f>(2*$Y65+1)*(2*$Y65+1)/($Z65*$AA65)</f>
+        <f t="shared" si="2"/>
         <v>144.5</v>
       </c>
       <c r="AI65">
@@ -37753,7 +39502,7 @@
         <v>10.676500000000001</v>
       </c>
       <c r="AQ65">
-        <f>(2*$AJ65+1)*(2*$AJ65+1)/($AK65*$AL65)</f>
+        <f t="shared" si="3"/>
         <v>144.5</v>
       </c>
       <c r="AT65">
@@ -37867,7 +39616,7 @@
         <v>6.1794500000000001</v>
       </c>
       <c r="AF66">
-        <f>(2*$Y66+1)*(2*$Y66+1)/($Z66*$AA66)</f>
+        <f t="shared" si="2"/>
         <v>144.5</v>
       </c>
       <c r="AI66">
@@ -37895,7 +39644,7 @@
         <v>8.7324800000000007</v>
       </c>
       <c r="AQ66">
-        <f>(2*$AJ66+1)*(2*$AJ66+1)/($AK66*$AL66)</f>
+        <f t="shared" si="3"/>
         <v>144.5</v>
       </c>
       <c r="AT66">
@@ -38009,7 +39758,7 @@
         <v>8.1810899999999993</v>
       </c>
       <c r="AF67">
-        <f>(2*$Y67+1)*(2*$Y67+1)/($Z67*$AA67)</f>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="AI67">
@@ -38037,7 +39786,7 @@
         <v>10.2895</v>
       </c>
       <c r="AQ67">
-        <f>(2*$AJ67+1)*(2*$AJ67+1)/($AK67*$AL67)</f>
+        <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="AT67">
@@ -38151,7 +39900,7 @@
         <v>7.9944600000000001</v>
       </c>
       <c r="AF68">
-        <f>(2*$Y68+1)*(2*$Y68+1)/($Z68*$AA68)</f>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
       <c r="AI68">
@@ -38179,7 +39928,7 @@
         <v>10.479799999999999</v>
       </c>
       <c r="AQ68">
-        <f>(2*$AJ68+1)*(2*$AJ68+1)/($AK68*$AL68)</f>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="AT68">
@@ -38293,7 +40042,7 @@
         <v>27.4163</v>
       </c>
       <c r="AF69">
-        <f>(2*$Y69+1)*(2*$Y69+1)/($Z69*$AA69)</f>
+        <f t="shared" ref="AF69:AF84" si="4">(2*$Y69+1)*(2*$Y69+1)/($Z69*$AA69)</f>
         <v>6.25</v>
       </c>
       <c r="AI69">
@@ -38321,7 +40070,7 @@
         <v>28.082899999999999</v>
       </c>
       <c r="AQ69">
-        <f>(2*$AJ69+1)*(2*$AJ69+1)/($AK69*$AL69)</f>
+        <f t="shared" ref="AQ69:AQ84" si="5">(2*$AJ69+1)*(2*$AJ69+1)/($AK69*$AL69)</f>
         <v>6.25</v>
       </c>
       <c r="AT69">
@@ -38435,7 +40184,7 @@
         <v>26.493500000000001</v>
       </c>
       <c r="AF70">
-        <f>(2*$Y70+1)*(2*$Y70+1)/($Z70*$AA70)</f>
+        <f t="shared" si="4"/>
         <v>12.5</v>
       </c>
       <c r="AI70">
@@ -38463,7 +40212,7 @@
         <v>25.4512</v>
       </c>
       <c r="AQ70">
-        <f>(2*$AJ70+1)*(2*$AJ70+1)/($AK70*$AL70)</f>
+        <f t="shared" si="5"/>
         <v>12.5</v>
       </c>
       <c r="AT70">
@@ -38583,7 +40332,7 @@
         <v>24.686299999999999</v>
       </c>
       <c r="AF71">
-        <f>(2*$Y71+1)*(2*$Y71+1)/($Z71*$AA71)</f>
+        <f t="shared" si="4"/>
         <v>12.5</v>
       </c>
       <c r="AI71">
@@ -38611,7 +40360,7 @@
         <v>27.206299999999999</v>
       </c>
       <c r="AQ71">
-        <f>(2*$AJ71+1)*(2*$AJ71+1)/($AK71*$AL71)</f>
+        <f t="shared" si="5"/>
         <v>12.5</v>
       </c>
       <c r="AT71">
@@ -38725,7 +40474,7 @@
         <v>16.177099999999999</v>
       </c>
       <c r="AF72">
-        <f>(2*$Y72+1)*(2*$Y72+1)/($Z72*$AA72)</f>
+        <f t="shared" si="4"/>
         <v>20.25</v>
       </c>
       <c r="AI72">
@@ -38753,7 +40502,7 @@
         <v>17.253299999999999</v>
       </c>
       <c r="AQ72">
-        <f>(2*$AJ72+1)*(2*$AJ72+1)/($AK72*$AL72)</f>
+        <f t="shared" si="5"/>
         <v>20.25</v>
       </c>
       <c r="AT72">
@@ -38867,7 +40616,7 @@
         <v>24.185500000000001</v>
       </c>
       <c r="AF73">
-        <f>(2*$Y73+1)*(2*$Y73+1)/($Z73*$AA73)</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="AG73" t="s">
@@ -38898,7 +40647,7 @@
         <v>24.985600000000002</v>
       </c>
       <c r="AQ73">
-        <f>(2*$AJ73+1)*(2*$AJ73+1)/($AK73*$AL73)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="AT73">
@@ -39012,7 +40761,7 @@
         <v>14.9627</v>
       </c>
       <c r="AF74">
-        <f>(2*$Y74+1)*(2*$Y74+1)/($Z74*$AA74)</f>
+        <f t="shared" si="4"/>
         <v>40.5</v>
       </c>
       <c r="AI74">
@@ -39040,7 +40789,7 @@
         <v>17.302199999999999</v>
       </c>
       <c r="AQ74">
-        <f>(2*$AJ74+1)*(2*$AJ74+1)/($AK74*$AL74)</f>
+        <f t="shared" si="5"/>
         <v>40.5</v>
       </c>
       <c r="AT74">
@@ -39154,7 +40903,7 @@
         <v>16.118400000000001</v>
       </c>
       <c r="AF75">
-        <f>(2*$Y75+1)*(2*$Y75+1)/($Z75*$AA75)</f>
+        <f t="shared" si="4"/>
         <v>40.5</v>
       </c>
       <c r="AI75">
@@ -39182,7 +40931,7 @@
         <v>16.096699999999998</v>
       </c>
       <c r="AQ75">
-        <f>(2*$AJ75+1)*(2*$AJ75+1)/($AK75*$AL75)</f>
+        <f t="shared" si="5"/>
         <v>40.5</v>
       </c>
       <c r="AT75">
@@ -39296,7 +41045,7 @@
         <v>12.791</v>
       </c>
       <c r="AF76">
-        <f>(2*$Y76+1)*(2*$Y76+1)/($Z76*$AA76)</f>
+        <f t="shared" si="4"/>
         <v>42.25</v>
       </c>
       <c r="AI76">
@@ -39324,7 +41073,7 @@
         <v>14.311999999999999</v>
       </c>
       <c r="AQ76">
-        <f>(2*$AJ76+1)*(2*$AJ76+1)/($AK76*$AL76)</f>
+        <f t="shared" si="5"/>
         <v>42.25</v>
       </c>
       <c r="AT76">
@@ -39438,7 +41187,7 @@
         <v>11.563599999999999</v>
       </c>
       <c r="AF77">
-        <f>(2*$Y77+1)*(2*$Y77+1)/($Z77*$AA77)</f>
+        <f t="shared" si="4"/>
         <v>72.25</v>
       </c>
       <c r="AI77">
@@ -39466,7 +41215,7 @@
         <v>13.514799999999999</v>
       </c>
       <c r="AQ77">
-        <f>(2*$AJ77+1)*(2*$AJ77+1)/($AK77*$AL77)</f>
+        <f t="shared" si="5"/>
         <v>72.25</v>
       </c>
       <c r="AT77">
@@ -39580,7 +41329,7 @@
         <v>15.157999999999999</v>
       </c>
       <c r="AF78">
-        <f>(2*$Y78+1)*(2*$Y78+1)/($Z78*$AA78)</f>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="AI78">
@@ -39608,7 +41357,7 @@
         <v>16.371200000000002</v>
       </c>
       <c r="AQ78">
-        <f>(2*$AJ78+1)*(2*$AJ78+1)/($AK78*$AL78)</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
       <c r="AT78">
@@ -39722,7 +41471,7 @@
         <v>13.740500000000001</v>
       </c>
       <c r="AF79">
-        <f>(2*$Y79+1)*(2*$Y79+1)/($Z79*$AA79)</f>
+        <f t="shared" si="4"/>
         <v>84.5</v>
       </c>
       <c r="AG79" t="s">
@@ -39753,7 +41502,7 @@
         <v>15.316000000000001</v>
       </c>
       <c r="AQ79">
-        <f>(2*$AJ79+1)*(2*$AJ79+1)/($AK79*$AL79)</f>
+        <f t="shared" si="5"/>
         <v>84.5</v>
       </c>
       <c r="AT79">
@@ -39867,7 +41616,7 @@
         <v>12.0006</v>
       </c>
       <c r="AF80">
-        <f>(2*$Y80+1)*(2*$Y80+1)/($Z80*$AA80)</f>
+        <f t="shared" si="4"/>
         <v>84.5</v>
       </c>
       <c r="AI80">
@@ -39895,7 +41644,7 @@
         <v>13.555400000000001</v>
       </c>
       <c r="AQ80">
-        <f>(2*$AJ80+1)*(2*$AJ80+1)/($AK80*$AL80)</f>
+        <f t="shared" si="5"/>
         <v>84.5</v>
       </c>
       <c r="AT80">
@@ -40009,7 +41758,7 @@
         <v>12.9427</v>
       </c>
       <c r="AF81">
-        <f>(2*$Y81+1)*(2*$Y81+1)/($Z81*$AA81)</f>
+        <f t="shared" si="4"/>
         <v>144.5</v>
       </c>
       <c r="AI81">
@@ -40037,7 +41786,7 @@
         <v>14.9079</v>
       </c>
       <c r="AQ81">
-        <f>(2*$AJ81+1)*(2*$AJ81+1)/($AK81*$AL81)</f>
+        <f t="shared" si="5"/>
         <v>144.5</v>
       </c>
       <c r="AT81">
@@ -40151,7 +41900,7 @@
         <v>11.0322</v>
       </c>
       <c r="AF82">
-        <f>(2*$Y82+1)*(2*$Y82+1)/($Z82*$AA82)</f>
+        <f t="shared" si="4"/>
         <v>144.5</v>
       </c>
       <c r="AI82">
@@ -40179,7 +41928,7 @@
         <v>12.996700000000001</v>
       </c>
       <c r="AQ82">
-        <f>(2*$AJ82+1)*(2*$AJ82+1)/($AK82*$AL82)</f>
+        <f t="shared" si="5"/>
         <v>144.5</v>
       </c>
       <c r="AT82">
@@ -40293,7 +42042,7 @@
         <v>13.081099999999999</v>
       </c>
       <c r="AF83">
-        <f>(2*$Y83+1)*(2*$Y83+1)/($Z83*$AA83)</f>
+        <f t="shared" si="4"/>
         <v>169</v>
       </c>
       <c r="AI83">
@@ -40321,7 +42070,7 @@
         <v>14.6694</v>
       </c>
       <c r="AQ83">
-        <f>(2*$AJ83+1)*(2*$AJ83+1)/($AK83*$AL83)</f>
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
       <c r="AT83">
@@ -40435,7 +42184,7 @@
         <v>12.465</v>
       </c>
       <c r="AF84">
-        <f>(2*$Y84+1)*(2*$Y84+1)/($Z84*$AA84)</f>
+        <f t="shared" si="4"/>
         <v>289</v>
       </c>
       <c r="AI84">
@@ -40463,7 +42212,7 @@
         <v>14.4299</v>
       </c>
       <c r="AQ84">
-        <f>(2*$AJ84+1)*(2*$AJ84+1)/($AK84*$AL84)</f>
+        <f t="shared" si="5"/>
         <v>289</v>
       </c>
       <c r="AT84">

</xml_diff>